<commit_message>
add nicaragua to data table 41
</commit_message>
<xml_diff>
--- a/data/t41_2000-2019.xlsx
+++ b/data/t41_2000-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\watti\OneDrive\Desktop\mit\11.154 datasets\11.154-proj-pathways\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F976E5-B53F-44D5-ADD0-FFCED05EAC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952E7254-2D64-4F3F-9D4A-DA970E813966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="1224" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table removals37" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
   <si>
     <t xml:space="preserve">Region and country of nationality  </t>
   </si>
@@ -149,6 +149,9 @@
       <t>1</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Nicaragua                          </t>
+  </si>
 </sst>
 </file>
 
@@ -158,10 +161,17 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -353,11 +363,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -413,13 +425,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -431,45 +475,32 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{7F6F3536-B3F6-47EF-894E-0705BCDCEDEA}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{646C8956-E82E-4A80-91BF-2BB897CE9D8E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -781,12 +812,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ80"/>
+  <dimension ref="A1:BJ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A143" sqref="A143"/>
-      <selection pane="topRight" activeCell="AI10" sqref="AI10"/>
+      <selection pane="topRight" activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -801,109 +832,109 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="29">
+      <c r="B1" s="47">
         <v>1999</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47">
         <v>2000</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29">
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47">
         <v>2001</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29">
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47">
         <v>2002</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29">
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47">
         <v>2003</v>
       </c>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29">
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47">
         <v>2004</v>
       </c>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29">
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47">
         <v>2005</v>
       </c>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29">
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47">
         <v>2006</v>
       </c>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29">
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47">
         <v>2007</v>
       </c>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="30">
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="44">
         <v>2008</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="46">
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="39">
         <v>2009</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AG1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="33" t="s">
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="33" t="s">
+      <c r="AK1" s="42"/>
+      <c r="AL1" s="43"/>
+      <c r="AM1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="35"/>
-      <c r="AP1" s="33" t="s">
+      <c r="AN1" s="42"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="35"/>
-      <c r="AS1" s="33" t="s">
+      <c r="AQ1" s="42"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="35"/>
-      <c r="AV1" s="33" t="s">
+      <c r="AT1" s="42"/>
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="33" t="s">
+      <c r="AW1" s="42"/>
+      <c r="AX1" s="43"/>
+      <c r="AY1" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="AZ1" s="34"/>
-      <c r="BA1" s="35"/>
-      <c r="BB1" s="34" t="s">
+      <c r="AZ1" s="42"/>
+      <c r="BA1" s="43"/>
+      <c r="BB1" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="35"/>
-      <c r="BE1" s="33" t="s">
+      <c r="BC1" s="42"/>
+      <c r="BD1" s="43"/>
+      <c r="BE1" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="35"/>
-      <c r="BH1" s="33" t="s">
+      <c r="BF1" s="42"/>
+      <c r="BG1" s="43"/>
+      <c r="BH1" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="35"/>
+      <c r="BI1" s="42"/>
+      <c r="BJ1" s="43"/>
     </row>
     <row r="2" spans="1:62" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
@@ -999,97 +1030,97 @@
       <c r="AE2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AF2" s="47" t="s">
+      <c r="AF2" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="36" t="s">
+      <c r="AG2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AH2" s="37" t="s">
+      <c r="AH2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="38" t="s">
+      <c r="AI2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AJ2" s="37" t="s">
+      <c r="AJ2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="37" t="s">
+      <c r="AK2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" s="37" t="s">
+      <c r="AL2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="AM2" s="36" t="s">
+      <c r="AM2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AN2" s="37" t="s">
+      <c r="AN2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AO2" s="38" t="s">
+      <c r="AO2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AP2" s="37" t="s">
+      <c r="AP2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="AQ2" s="37" t="s">
+      <c r="AQ2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AR2" s="37" t="s">
+      <c r="AR2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="AS2" s="36" t="s">
+      <c r="AS2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AT2" s="37" t="s">
+      <c r="AT2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AU2" s="38" t="s">
+      <c r="AU2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AV2" s="37" t="s">
+      <c r="AV2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="AW2" s="37" t="s">
+      <c r="AW2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AX2" s="37" t="s">
+      <c r="AX2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="AY2" s="36" t="s">
+      <c r="AY2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AZ2" s="37" t="s">
+      <c r="AZ2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="BA2" s="38" t="s">
+      <c r="BA2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="BB2" s="37" t="s">
+      <c r="BB2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="BC2" s="37" t="s">
+      <c r="BC2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="BD2" s="38" t="s">
+      <c r="BD2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="BE2" s="36" t="s">
+      <c r="BE2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="BF2" s="37" t="s">
+      <c r="BF2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="BG2" s="38" t="s">
+      <c r="BG2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="BH2" s="36" t="s">
+      <c r="BH2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="BI2" s="37" t="s">
+      <c r="BI2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="BJ2" s="38" t="s">
+      <c r="BJ2" s="31" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1136,36 +1167,36 @@
       <c r="AF3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AG3" s="39"/>
-      <c r="AH3" s="39"/>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="39"/>
-      <c r="AK3" s="39"/>
-      <c r="AL3" s="40"/>
-      <c r="AM3" s="39"/>
-      <c r="AN3" s="39"/>
-      <c r="AO3" s="40"/>
-      <c r="AP3" s="39"/>
-      <c r="AQ3" s="39"/>
-      <c r="AR3" s="40"/>
-      <c r="AS3" s="39"/>
-      <c r="AT3" s="39"/>
-      <c r="AU3" s="40"/>
-      <c r="AV3" s="39"/>
-      <c r="AW3" s="39"/>
-      <c r="AX3" s="40"/>
-      <c r="AY3" s="39"/>
-      <c r="AZ3" s="39"/>
-      <c r="BA3" s="40"/>
-      <c r="BB3" s="39"/>
-      <c r="BC3" s="39"/>
-      <c r="BD3" s="40"/>
-      <c r="BE3" s="39"/>
-      <c r="BF3" s="39"/>
-      <c r="BG3" s="40"/>
-      <c r="BH3" s="39"/>
-      <c r="BI3" s="39"/>
-      <c r="BJ3" s="40"/>
+      <c r="AG3" s="32"/>
+      <c r="AH3" s="32"/>
+      <c r="AI3" s="33"/>
+      <c r="AJ3" s="32"/>
+      <c r="AK3" s="32"/>
+      <c r="AL3" s="33"/>
+      <c r="AM3" s="32"/>
+      <c r="AN3" s="32"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="32"/>
+      <c r="AQ3" s="32"/>
+      <c r="AR3" s="33"/>
+      <c r="AS3" s="32"/>
+      <c r="AT3" s="32"/>
+      <c r="AU3" s="33"/>
+      <c r="AV3" s="32"/>
+      <c r="AW3" s="32"/>
+      <c r="AX3" s="33"/>
+      <c r="AY3" s="32"/>
+      <c r="AZ3" s="32"/>
+      <c r="BA3" s="33"/>
+      <c r="BB3" s="32"/>
+      <c r="BC3" s="32"/>
+      <c r="BD3" s="33"/>
+      <c r="BE3" s="32"/>
+      <c r="BF3" s="32"/>
+      <c r="BG3" s="33"/>
+      <c r="BH3" s="32"/>
+      <c r="BI3" s="32"/>
+      <c r="BJ3" s="33"/>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1264,94 +1295,94 @@
       <c r="AF4" s="27">
         <v>580107</v>
       </c>
-      <c r="AG4" s="39">
+      <c r="AG4" s="32">
         <v>382449</v>
       </c>
-      <c r="AH4" s="39">
+      <c r="AH4" s="32">
         <v>171030</v>
       </c>
-      <c r="AI4" s="41">
+      <c r="AI4" s="34">
         <v>211419</v>
       </c>
-      <c r="AJ4" s="39">
+      <c r="AJ4" s="32">
         <v>390423</v>
       </c>
-      <c r="AK4" s="39">
+      <c r="AK4" s="32">
         <v>189702</v>
       </c>
-      <c r="AL4" s="41">
+      <c r="AL4" s="34">
         <v>200721</v>
       </c>
-      <c r="AM4" s="39">
+      <c r="AM4" s="32">
         <v>415607</v>
       </c>
-      <c r="AN4" s="39">
+      <c r="AN4" s="32">
         <v>200039</v>
       </c>
-      <c r="AO4" s="41">
+      <c r="AO4" s="34">
         <v>215568</v>
       </c>
-      <c r="AP4" s="39">
+      <c r="AP4" s="32">
         <v>432228</v>
       </c>
-      <c r="AQ4" s="39">
+      <c r="AQ4" s="32">
         <v>198488</v>
       </c>
-      <c r="AR4" s="41">
+      <c r="AR4" s="34">
         <v>233740</v>
       </c>
-      <c r="AS4" s="39">
+      <c r="AS4" s="32">
         <v>405090</v>
       </c>
-      <c r="AT4" s="39">
+      <c r="AT4" s="32">
         <v>169459</v>
       </c>
-      <c r="AU4" s="41">
+      <c r="AU4" s="34">
         <v>235631</v>
       </c>
-      <c r="AV4" s="39">
+      <c r="AV4" s="32">
         <v>325328</v>
       </c>
-      <c r="AW4" s="39">
+      <c r="AW4" s="32">
         <v>120846</v>
       </c>
-      <c r="AX4" s="41">
+      <c r="AX4" s="34">
         <v>204482</v>
       </c>
-      <c r="AY4" s="39">
+      <c r="AY4" s="32">
         <v>331717</v>
       </c>
-      <c r="AZ4" s="39">
+      <c r="AZ4" s="32">
         <v>115301</v>
       </c>
-      <c r="BA4" s="41">
+      <c r="BA4" s="34">
         <v>216416</v>
       </c>
-      <c r="BB4" s="39">
+      <c r="BB4" s="32">
         <v>287093</v>
       </c>
-      <c r="BC4" s="39">
+      <c r="BC4" s="32">
         <v>109697</v>
       </c>
-      <c r="BD4" s="41">
+      <c r="BD4" s="34">
         <v>177396</v>
       </c>
-      <c r="BE4" s="39">
+      <c r="BE4" s="32">
         <v>328716</v>
       </c>
-      <c r="BF4" s="39">
+      <c r="BF4" s="32">
         <v>148352</v>
       </c>
-      <c r="BG4" s="41">
+      <c r="BG4" s="34">
         <v>180364</v>
       </c>
-      <c r="BH4" s="39">
+      <c r="BH4" s="32">
         <v>359885</v>
       </c>
-      <c r="BI4" s="39">
+      <c r="BI4" s="32">
         <v>155788</v>
       </c>
-      <c r="BJ4" s="41">
+      <c r="BJ4" s="34">
         <v>204097</v>
       </c>
     </row>
@@ -1452,94 +1483,94 @@
       <c r="AF5" s="27">
         <v>3047</v>
       </c>
-      <c r="AG5" s="39">
+      <c r="AG5" s="32">
         <v>1773</v>
       </c>
-      <c r="AH5" s="39">
+      <c r="AH5" s="32">
         <v>675</v>
       </c>
-      <c r="AI5" s="41">
+      <c r="AI5" s="34">
         <v>1098</v>
       </c>
-      <c r="AJ5" s="39">
+      <c r="AJ5" s="32">
         <v>1865</v>
       </c>
-      <c r="AK5" s="39">
+      <c r="AK5" s="32">
         <v>663</v>
       </c>
-      <c r="AL5" s="41">
+      <c r="AL5" s="34">
         <v>1202</v>
       </c>
-      <c r="AM5" s="39">
+      <c r="AM5" s="32">
         <v>1427</v>
       </c>
-      <c r="AN5" s="39">
+      <c r="AN5" s="32">
         <v>668</v>
       </c>
-      <c r="AO5" s="41">
+      <c r="AO5" s="34">
         <v>759</v>
       </c>
-      <c r="AP5" s="39">
+      <c r="AP5" s="32">
         <v>1288</v>
       </c>
-      <c r="AQ5" s="39">
+      <c r="AQ5" s="32">
         <v>605</v>
       </c>
-      <c r="AR5" s="41">
+      <c r="AR5" s="34">
         <v>683</v>
       </c>
-      <c r="AS5" s="39">
+      <c r="AS5" s="32">
         <v>1285</v>
       </c>
-      <c r="AT5" s="39">
+      <c r="AT5" s="32">
         <v>528</v>
       </c>
-      <c r="AU5" s="41">
+      <c r="AU5" s="34">
         <v>757</v>
       </c>
-      <c r="AV5" s="39">
+      <c r="AV5" s="32">
         <v>1362</v>
       </c>
-      <c r="AW5" s="39">
+      <c r="AW5" s="32">
         <v>376</v>
       </c>
-      <c r="AX5" s="41">
+      <c r="AX5" s="34">
         <v>986</v>
       </c>
-      <c r="AY5" s="39">
+      <c r="AY5" s="32">
         <v>1521</v>
       </c>
-      <c r="AZ5" s="39">
+      <c r="AZ5" s="32">
         <v>409</v>
       </c>
-      <c r="BA5" s="41">
+      <c r="BA5" s="34">
         <v>1112</v>
       </c>
-      <c r="BB5" s="39">
+      <c r="BB5" s="32">
         <v>2946</v>
       </c>
-      <c r="BC5" s="39">
+      <c r="BC5" s="32">
         <v>887</v>
       </c>
-      <c r="BD5" s="41">
+      <c r="BD5" s="34">
         <v>2059</v>
       </c>
-      <c r="BE5" s="39">
+      <c r="BE5" s="32">
         <v>3332</v>
       </c>
-      <c r="BF5" s="39">
+      <c r="BF5" s="32">
         <v>2009</v>
       </c>
-      <c r="BG5" s="41">
+      <c r="BG5" s="34">
         <v>1323</v>
       </c>
-      <c r="BH5" s="39">
+      <c r="BH5" s="32">
         <v>2601</v>
       </c>
-      <c r="BI5" s="39">
+      <c r="BI5" s="32">
         <v>1747</v>
       </c>
-      <c r="BJ5" s="41">
+      <c r="BJ5" s="34">
         <v>854</v>
       </c>
     </row>
@@ -1640,94 +1671,94 @@
       <c r="AF6" s="27">
         <v>53885</v>
       </c>
-      <c r="AG6" s="39">
+      <c r="AG6" s="32">
         <v>5647</v>
       </c>
-      <c r="AH6" s="39">
+      <c r="AH6" s="32">
         <v>1529</v>
       </c>
-      <c r="AI6" s="41">
+      <c r="AI6" s="34">
         <v>4118</v>
       </c>
-      <c r="AJ6" s="39">
+      <c r="AJ6" s="32">
         <v>6155</v>
       </c>
-      <c r="AK6" s="39">
+      <c r="AK6" s="32">
         <v>1626</v>
       </c>
-      <c r="AL6" s="41">
+      <c r="AL6" s="34">
         <v>4529</v>
       </c>
-      <c r="AM6" s="39">
+      <c r="AM6" s="32">
         <v>4293</v>
       </c>
-      <c r="AN6" s="39">
+      <c r="AN6" s="32">
         <v>1466</v>
       </c>
-      <c r="AO6" s="41">
+      <c r="AO6" s="34">
         <v>2827</v>
       </c>
-      <c r="AP6" s="39">
+      <c r="AP6" s="32">
         <v>3475</v>
       </c>
-      <c r="AQ6" s="39">
+      <c r="AQ6" s="32">
         <v>1153</v>
       </c>
-      <c r="AR6" s="41">
+      <c r="AR6" s="34">
         <v>2322</v>
       </c>
-      <c r="AS6" s="39">
+      <c r="AS6" s="32">
         <v>2984</v>
       </c>
-      <c r="AT6" s="39">
+      <c r="AT6" s="32">
         <v>1092</v>
       </c>
-      <c r="AU6" s="41">
+      <c r="AU6" s="34">
         <v>1892</v>
       </c>
-      <c r="AV6" s="39">
+      <c r="AV6" s="32">
         <v>2639</v>
       </c>
-      <c r="AW6" s="39">
+      <c r="AW6" s="32">
         <v>806</v>
       </c>
-      <c r="AX6" s="41">
+      <c r="AX6" s="34">
         <v>1833</v>
       </c>
-      <c r="AY6" s="39">
+      <c r="AY6" s="32">
         <v>3313</v>
       </c>
-      <c r="AZ6" s="39">
+      <c r="AZ6" s="32">
         <v>792</v>
       </c>
-      <c r="BA6" s="41">
+      <c r="BA6" s="34">
         <v>2521</v>
       </c>
-      <c r="BB6" s="39">
+      <c r="BB6" s="32">
         <v>4896</v>
       </c>
-      <c r="BC6" s="39">
+      <c r="BC6" s="32">
         <v>957</v>
       </c>
-      <c r="BD6" s="41">
+      <c r="BD6" s="34">
         <v>3939</v>
       </c>
-      <c r="BE6" s="39">
+      <c r="BE6" s="32">
         <v>4528</v>
       </c>
-      <c r="BF6" s="39">
+      <c r="BF6" s="32">
         <v>2852</v>
       </c>
-      <c r="BG6" s="41">
+      <c r="BG6" s="34">
         <v>1676</v>
       </c>
-      <c r="BH6" s="39">
+      <c r="BH6" s="32">
         <v>6296</v>
       </c>
-      <c r="BI6" s="39">
+      <c r="BI6" s="32">
         <v>3688</v>
       </c>
-      <c r="BJ6" s="41">
+      <c r="BJ6" s="34">
         <v>2608</v>
       </c>
     </row>
@@ -2024,94 +2055,94 @@
       <c r="AF9" s="27">
         <v>20611</v>
       </c>
-      <c r="AG9" s="39">
+      <c r="AG9" s="32">
         <v>4045</v>
       </c>
-      <c r="AH9" s="39">
+      <c r="AH9" s="32">
         <v>1259</v>
       </c>
-      <c r="AI9" s="41">
+      <c r="AI9" s="34">
         <v>2786</v>
       </c>
-      <c r="AJ9" s="39">
+      <c r="AJ9" s="32">
         <v>3475</v>
       </c>
-      <c r="AK9" s="39">
+      <c r="AK9" s="32">
         <v>1275</v>
       </c>
-      <c r="AL9" s="41">
+      <c r="AL9" s="34">
         <v>2200</v>
       </c>
-      <c r="AM9" s="39">
+      <c r="AM9" s="32">
         <v>2799</v>
       </c>
-      <c r="AN9" s="39">
+      <c r="AN9" s="32">
         <v>1266</v>
       </c>
-      <c r="AO9" s="41">
+      <c r="AO9" s="34">
         <v>1533</v>
       </c>
-      <c r="AP9" s="39">
+      <c r="AP9" s="32">
         <v>2162</v>
       </c>
-      <c r="AQ9" s="39">
+      <c r="AQ9" s="32">
         <v>1100</v>
       </c>
-      <c r="AR9" s="41">
+      <c r="AR9" s="34">
         <v>1062</v>
       </c>
-      <c r="AS9" s="39">
+      <c r="AS9" s="32">
         <v>1758</v>
       </c>
-      <c r="AT9" s="39">
+      <c r="AT9" s="32">
         <v>889</v>
       </c>
-      <c r="AU9" s="41">
+      <c r="AU9" s="34">
         <v>869</v>
       </c>
-      <c r="AV9" s="39">
+      <c r="AV9" s="32">
         <v>1463</v>
       </c>
-      <c r="AW9" s="39">
+      <c r="AW9" s="32">
         <v>722</v>
       </c>
-      <c r="AX9" s="41">
+      <c r="AX9" s="34">
         <v>741</v>
       </c>
-      <c r="AY9" s="39">
+      <c r="AY9" s="32">
         <v>1494</v>
       </c>
-      <c r="AZ9" s="39">
+      <c r="AZ9" s="32">
         <v>680</v>
       </c>
-      <c r="BA9" s="41">
+      <c r="BA9" s="34">
         <v>814</v>
       </c>
-      <c r="BB9" s="39">
+      <c r="BB9" s="32">
         <v>2015</v>
       </c>
-      <c r="BC9" s="39">
+      <c r="BC9" s="32">
         <v>796</v>
       </c>
-      <c r="BD9" s="41">
+      <c r="BD9" s="34">
         <v>1219</v>
       </c>
-      <c r="BE9" s="39">
+      <c r="BE9" s="32">
         <v>2480</v>
       </c>
-      <c r="BF9" s="39">
+      <c r="BF9" s="32">
         <v>1340</v>
       </c>
-      <c r="BG9" s="41">
+      <c r="BG9" s="34">
         <v>1140</v>
       </c>
-      <c r="BH9" s="39">
+      <c r="BH9" s="32">
         <v>2494</v>
       </c>
-      <c r="BI9" s="39">
+      <c r="BI9" s="32">
         <v>1399</v>
       </c>
-      <c r="BJ9" s="41">
+      <c r="BJ9" s="34">
         <v>1095</v>
       </c>
     </row>
@@ -2212,94 +2243,94 @@
       <c r="AF10" s="27">
         <v>490581</v>
       </c>
-      <c r="AG10" s="39">
+      <c r="AG10" s="32">
         <v>360039</v>
       </c>
-      <c r="AH10" s="39">
+      <c r="AH10" s="32">
         <v>163835</v>
       </c>
-      <c r="AI10" s="41">
+      <c r="AI10" s="34">
         <v>196204</v>
       </c>
-      <c r="AJ10" s="39">
+      <c r="AJ10" s="32">
         <v>368643</v>
       </c>
-      <c r="AK10" s="39">
+      <c r="AK10" s="32">
         <v>182471</v>
       </c>
-      <c r="AL10" s="41">
+      <c r="AL10" s="34">
         <v>186172</v>
       </c>
-      <c r="AM10" s="39">
+      <c r="AM10" s="32">
         <v>398832</v>
       </c>
-      <c r="AN10" s="39">
+      <c r="AN10" s="32">
         <v>193231</v>
       </c>
-      <c r="AO10" s="41">
+      <c r="AO10" s="34">
         <v>205601</v>
       </c>
-      <c r="AP10" s="39">
+      <c r="AP10" s="32">
         <v>418933</v>
       </c>
-      <c r="AQ10" s="39">
+      <c r="AQ10" s="32">
         <v>192716</v>
       </c>
-      <c r="AR10" s="41">
+      <c r="AR10" s="34">
         <v>226217</v>
       </c>
-      <c r="AS10" s="39">
+      <c r="AS10" s="32">
         <v>393526</v>
       </c>
-      <c r="AT10" s="39">
+      <c r="AT10" s="32">
         <v>164307</v>
       </c>
-      <c r="AU10" s="41">
+      <c r="AU10" s="34">
         <v>229219</v>
       </c>
-      <c r="AV10" s="39">
+      <c r="AV10" s="32">
         <v>314403</v>
       </c>
-      <c r="AW10" s="39">
+      <c r="AW10" s="32">
         <v>116682</v>
       </c>
-      <c r="AX10" s="41">
+      <c r="AX10" s="34">
         <v>197721</v>
       </c>
-      <c r="AY10" s="39">
+      <c r="AY10" s="32">
         <v>318260</v>
       </c>
-      <c r="AZ10" s="39">
+      <c r="AZ10" s="32">
         <v>111193</v>
       </c>
-      <c r="BA10" s="41">
+      <c r="BA10" s="34">
         <v>207067</v>
       </c>
-      <c r="BB10" s="39">
+      <c r="BB10" s="32">
         <v>269302</v>
       </c>
-      <c r="BC10" s="39">
+      <c r="BC10" s="32">
         <v>104761</v>
       </c>
-      <c r="BD10" s="41">
+      <c r="BD10" s="34">
         <v>164541</v>
       </c>
-      <c r="BE10" s="39">
+      <c r="BE10" s="32">
         <v>308744</v>
       </c>
-      <c r="BF10" s="39">
+      <c r="BF10" s="32">
         <v>135015</v>
       </c>
-      <c r="BG10" s="41">
+      <c r="BG10" s="34">
         <v>173729</v>
       </c>
-      <c r="BH10" s="39">
+      <c r="BH10" s="32">
         <v>336824</v>
       </c>
-      <c r="BI10" s="39">
+      <c r="BI10" s="32">
         <v>140181</v>
       </c>
-      <c r="BJ10" s="41">
+      <c r="BJ10" s="34">
         <v>196643</v>
       </c>
     </row>
@@ -2400,94 +2431,94 @@
       <c r="AF11" s="27">
         <v>1130</v>
       </c>
-      <c r="AG11" s="39">
+      <c r="AG11" s="32">
         <v>308</v>
       </c>
-      <c r="AH11" s="39">
+      <c r="AH11" s="32">
         <v>200</v>
       </c>
-      <c r="AI11" s="41">
+      <c r="AI11" s="34">
         <v>108</v>
       </c>
-      <c r="AJ11" s="39">
+      <c r="AJ11" s="32">
         <v>334</v>
       </c>
-      <c r="AK11" s="39">
+      <c r="AK11" s="32">
         <v>222</v>
       </c>
-      <c r="AL11" s="41">
+      <c r="AL11" s="34">
         <v>112</v>
       </c>
-      <c r="AM11" s="39">
+      <c r="AM11" s="32">
         <v>256</v>
       </c>
-      <c r="AN11" s="39">
+      <c r="AN11" s="32">
         <v>189</v>
       </c>
-      <c r="AO11" s="41">
+      <c r="AO11" s="34">
         <v>67</v>
       </c>
-      <c r="AP11" s="39">
+      <c r="AP11" s="32">
         <v>238</v>
       </c>
-      <c r="AQ11" s="39">
+      <c r="AQ11" s="32">
         <v>192</v>
       </c>
-      <c r="AR11" s="41">
+      <c r="AR11" s="34">
         <v>46</v>
       </c>
-      <c r="AS11" s="39">
+      <c r="AS11" s="32">
         <v>228</v>
       </c>
-      <c r="AT11" s="39">
+      <c r="AT11" s="32">
         <v>184</v>
       </c>
-      <c r="AU11" s="41">
+      <c r="AU11" s="34">
         <v>44</v>
       </c>
-      <c r="AV11" s="39">
+      <c r="AV11" s="32">
         <v>185</v>
       </c>
-      <c r="AW11" s="39">
+      <c r="AW11" s="32">
         <v>149</v>
       </c>
-      <c r="AX11" s="41">
+      <c r="AX11" s="34">
         <v>36</v>
       </c>
-      <c r="AY11" s="39">
+      <c r="AY11" s="32">
         <v>237</v>
       </c>
-      <c r="AZ11" s="39">
+      <c r="AZ11" s="32">
         <v>162</v>
       </c>
-      <c r="BA11" s="41">
+      <c r="BA11" s="34">
         <v>75</v>
       </c>
-      <c r="BB11" s="39">
+      <c r="BB11" s="32">
         <v>276</v>
       </c>
-      <c r="BC11" s="39">
+      <c r="BC11" s="32">
         <v>186</v>
       </c>
-      <c r="BD11" s="41">
+      <c r="BD11" s="34">
         <v>90</v>
       </c>
-      <c r="BE11" s="39">
+      <c r="BE11" s="32">
         <v>323</v>
       </c>
-      <c r="BF11" s="39">
+      <c r="BF11" s="32">
         <v>289</v>
       </c>
-      <c r="BG11" s="41">
+      <c r="BG11" s="34">
         <v>34</v>
       </c>
-      <c r="BH11" s="39">
+      <c r="BH11" s="32">
         <v>288</v>
       </c>
-      <c r="BI11" s="39">
+      <c r="BI11" s="32">
         <v>262</v>
       </c>
-      <c r="BJ11" s="41">
+      <c r="BJ11" s="34">
         <v>26</v>
       </c>
     </row>
@@ -2588,94 +2619,94 @@
       <c r="AF12" s="27">
         <v>3499</v>
       </c>
-      <c r="AG12" s="39">
+      <c r="AG12" s="32">
         <v>10576</v>
       </c>
-      <c r="AH12" s="39">
+      <c r="AH12" s="32">
         <v>3515</v>
       </c>
-      <c r="AI12" s="41">
+      <c r="AI12" s="34">
         <v>7061</v>
       </c>
-      <c r="AJ12" s="39">
+      <c r="AJ12" s="32">
         <v>9869</v>
       </c>
-      <c r="AK12" s="39">
+      <c r="AK12" s="32">
         <v>3430</v>
       </c>
-      <c r="AL12" s="41">
+      <c r="AL12" s="34">
         <v>6439</v>
       </c>
-      <c r="AM12" s="39">
+      <c r="AM12" s="32">
         <v>7968</v>
       </c>
-      <c r="AN12" s="39">
+      <c r="AN12" s="32">
         <v>3207</v>
       </c>
-      <c r="AO12" s="41">
+      <c r="AO12" s="34">
         <v>4761</v>
       </c>
-      <c r="AP12" s="39">
+      <c r="AP12" s="32">
         <v>6095</v>
       </c>
-      <c r="AQ12" s="39">
+      <c r="AQ12" s="32">
         <v>2705</v>
       </c>
-      <c r="AR12" s="41">
+      <c r="AR12" s="34">
         <v>3390</v>
       </c>
-      <c r="AS12" s="39">
+      <c r="AS12" s="32">
         <v>5287</v>
       </c>
-      <c r="AT12" s="39">
+      <c r="AT12" s="32">
         <v>2450</v>
       </c>
-      <c r="AU12" s="41">
+      <c r="AU12" s="34">
         <v>2837</v>
       </c>
-      <c r="AV12" s="39">
+      <c r="AV12" s="32">
         <v>5239</v>
       </c>
-      <c r="AW12" s="39">
+      <c r="AW12" s="32">
         <v>2099</v>
       </c>
-      <c r="AX12" s="41">
+      <c r="AX12" s="34">
         <v>3140</v>
       </c>
-      <c r="AY12" s="39">
+      <c r="AY12" s="32">
         <v>6857</v>
       </c>
-      <c r="AZ12" s="39">
+      <c r="AZ12" s="32">
         <v>2058</v>
       </c>
-      <c r="BA12" s="41">
+      <c r="BA12" s="34">
         <v>4799</v>
       </c>
-      <c r="BB12" s="39">
+      <c r="BB12" s="32">
         <v>7622</v>
       </c>
-      <c r="BC12" s="39">
+      <c r="BC12" s="32">
         <v>2106</v>
       </c>
-      <c r="BD12" s="41">
+      <c r="BD12" s="34">
         <v>5516</v>
       </c>
-      <c r="BE12" s="39">
+      <c r="BE12" s="32">
         <v>9253</v>
       </c>
-      <c r="BF12" s="39">
+      <c r="BF12" s="32">
         <v>6813</v>
       </c>
-      <c r="BG12" s="41">
+      <c r="BG12" s="34">
         <v>2440</v>
       </c>
-      <c r="BH12" s="39">
+      <c r="BH12" s="32">
         <v>11338</v>
       </c>
-      <c r="BI12" s="39">
+      <c r="BI12" s="32">
         <v>8480</v>
       </c>
-      <c r="BJ12" s="41">
+      <c r="BJ12" s="34">
         <v>2858</v>
       </c>
     </row>
@@ -2776,94 +2807,94 @@
       <c r="AF13" s="28">
         <v>178</v>
       </c>
-      <c r="AG13" s="42">
+      <c r="AG13" s="35">
         <v>61</v>
       </c>
-      <c r="AH13" s="42">
+      <c r="AH13" s="35">
         <v>17</v>
       </c>
-      <c r="AI13" s="43">
+      <c r="AI13" s="36">
         <v>44</v>
       </c>
-      <c r="AJ13" s="42">
+      <c r="AJ13" s="35">
         <v>82</v>
       </c>
-      <c r="AK13" s="42">
+      <c r="AK13" s="35">
         <v>15</v>
       </c>
-      <c r="AL13" s="43">
+      <c r="AL13" s="36">
         <v>67</v>
       </c>
-      <c r="AM13" s="42">
+      <c r="AM13" s="35">
         <v>32</v>
       </c>
-      <c r="AN13" s="42">
+      <c r="AN13" s="35">
         <v>12</v>
       </c>
-      <c r="AO13" s="43">
+      <c r="AO13" s="36">
         <v>20</v>
       </c>
-      <c r="AP13" s="42">
+      <c r="AP13" s="35">
         <v>37</v>
       </c>
-      <c r="AQ13" s="42">
+      <c r="AQ13" s="35">
         <v>17</v>
       </c>
-      <c r="AR13" s="43">
+      <c r="AR13" s="36">
         <v>20</v>
       </c>
-      <c r="AS13" s="42">
+      <c r="AS13" s="35">
         <v>22</v>
       </c>
-      <c r="AT13" s="42">
+      <c r="AT13" s="35">
         <v>9</v>
       </c>
-      <c r="AU13" s="43">
+      <c r="AU13" s="36">
         <v>13</v>
       </c>
-      <c r="AV13" s="42">
+      <c r="AV13" s="35">
         <v>37</v>
       </c>
-      <c r="AW13" s="42">
+      <c r="AW13" s="35">
         <v>12</v>
       </c>
-      <c r="AX13" s="43">
+      <c r="AX13" s="36">
         <v>25</v>
       </c>
-      <c r="AY13" s="42">
+      <c r="AY13" s="35">
         <v>35</v>
       </c>
-      <c r="AZ13" s="42">
+      <c r="AZ13" s="35">
         <v>7</v>
       </c>
-      <c r="BA13" s="43">
+      <c r="BA13" s="36">
         <v>28</v>
       </c>
-      <c r="BB13" s="42">
+      <c r="BB13" s="35">
         <v>36</v>
       </c>
-      <c r="BC13" s="42">
+      <c r="BC13" s="35">
         <v>4</v>
       </c>
-      <c r="BD13" s="43">
+      <c r="BD13" s="36">
         <v>32</v>
       </c>
-      <c r="BE13" s="42">
+      <c r="BE13" s="35">
         <v>56</v>
       </c>
-      <c r="BF13" s="42">
+      <c r="BF13" s="35">
         <v>34</v>
       </c>
-      <c r="BG13" s="43">
+      <c r="BG13" s="36">
         <v>22</v>
       </c>
-      <c r="BH13" s="42">
+      <c r="BH13" s="35">
         <v>44</v>
       </c>
-      <c r="BI13" s="42">
+      <c r="BI13" s="35">
         <v>31</v>
       </c>
-      <c r="BJ13" s="43">
+      <c r="BJ13" s="36">
         <v>13</v>
       </c>
     </row>
@@ -2964,94 +2995,94 @@
       <c r="AF14" s="27">
         <v>63</v>
       </c>
-      <c r="AG14" s="44">
+      <c r="AG14" s="37">
         <v>254</v>
       </c>
-      <c r="AH14" s="44">
+      <c r="AH14" s="37">
         <v>157</v>
       </c>
-      <c r="AI14" s="45">
+      <c r="AI14" s="38">
         <v>97</v>
       </c>
-      <c r="AJ14" s="44">
+      <c r="AJ14" s="37">
         <v>221</v>
       </c>
-      <c r="AK14" s="44">
+      <c r="AK14" s="37">
         <v>158</v>
       </c>
-      <c r="AL14" s="45">
+      <c r="AL14" s="38">
         <v>63</v>
       </c>
-      <c r="AM14" s="44">
+      <c r="AM14" s="37">
         <v>204</v>
       </c>
-      <c r="AN14" s="44">
+      <c r="AN14" s="37">
         <v>146</v>
       </c>
-      <c r="AO14" s="45">
+      <c r="AO14" s="38">
         <v>58</v>
       </c>
-      <c r="AP14" s="44">
+      <c r="AP14" s="37">
         <v>175</v>
       </c>
-      <c r="AQ14" s="44">
+      <c r="AQ14" s="37">
         <v>121</v>
       </c>
-      <c r="AR14" s="45">
+      <c r="AR14" s="38">
         <v>54</v>
       </c>
-      <c r="AS14" s="44">
+      <c r="AS14" s="37">
         <v>136</v>
       </c>
-      <c r="AT14" s="44">
+      <c r="AT14" s="37">
         <v>79</v>
       </c>
-      <c r="AU14" s="45">
+      <c r="AU14" s="38">
         <v>57</v>
       </c>
-      <c r="AV14" s="44">
+      <c r="AV14" s="37">
         <v>134</v>
       </c>
-      <c r="AW14" s="44">
+      <c r="AW14" s="37">
         <v>83</v>
       </c>
-      <c r="AX14" s="45">
+      <c r="AX14" s="38">
         <v>51</v>
       </c>
-      <c r="AY14" s="44">
+      <c r="AY14" s="37">
         <v>146</v>
       </c>
-      <c r="AZ14" s="44">
+      <c r="AZ14" s="37">
         <v>86</v>
       </c>
-      <c r="BA14" s="45">
+      <c r="BA14" s="38">
         <v>60</v>
       </c>
-      <c r="BB14" s="44">
+      <c r="BB14" s="37">
         <v>123</v>
       </c>
-      <c r="BC14" s="44">
+      <c r="BC14" s="37">
         <v>57</v>
       </c>
-      <c r="BD14" s="45">
+      <c r="BD14" s="38">
         <v>66</v>
       </c>
-      <c r="BE14" s="44">
+      <c r="BE14" s="37">
         <v>133</v>
       </c>
-      <c r="BF14" s="44">
+      <c r="BF14" s="37">
         <v>111</v>
       </c>
-      <c r="BG14" s="45">
+      <c r="BG14" s="38">
         <v>22</v>
       </c>
-      <c r="BH14" s="44">
+      <c r="BH14" s="37">
         <v>109</v>
       </c>
-      <c r="BI14" s="44">
+      <c r="BI14" s="37">
         <v>80</v>
       </c>
-      <c r="BJ14" s="45">
+      <c r="BJ14" s="38">
         <v>29</v>
       </c>
     </row>
@@ -3152,94 +3183,94 @@
       <c r="AF15" s="27">
         <v>152</v>
       </c>
-      <c r="AG15" s="44">
+      <c r="AG15" s="37">
         <v>558</v>
       </c>
-      <c r="AH15" s="44">
+      <c r="AH15" s="37">
         <v>159</v>
       </c>
-      <c r="AI15" s="45">
+      <c r="AI15" s="38">
         <v>399</v>
       </c>
-      <c r="AJ15" s="44">
+      <c r="AJ15" s="37">
         <v>415</v>
       </c>
-      <c r="AK15" s="44">
+      <c r="AK15" s="37">
         <v>161</v>
       </c>
-      <c r="AL15" s="45">
+      <c r="AL15" s="38">
         <v>254</v>
       </c>
-      <c r="AM15" s="44">
+      <c r="AM15" s="37">
         <v>398</v>
       </c>
-      <c r="AN15" s="44">
+      <c r="AN15" s="37">
         <v>131</v>
       </c>
-      <c r="AO15" s="45">
+      <c r="AO15" s="38">
         <v>267</v>
       </c>
-      <c r="AP15" s="44">
+      <c r="AP15" s="37">
         <v>332</v>
       </c>
-      <c r="AQ15" s="44">
+      <c r="AQ15" s="37">
         <v>128</v>
       </c>
-      <c r="AR15" s="45">
+      <c r="AR15" s="38">
         <v>204</v>
       </c>
-      <c r="AS15" s="44">
+      <c r="AS15" s="37">
         <v>286</v>
       </c>
-      <c r="AT15" s="44">
+      <c r="AT15" s="37">
         <v>125</v>
       </c>
-      <c r="AU15" s="45">
+      <c r="AU15" s="38">
         <v>161</v>
       </c>
-      <c r="AV15" s="44">
+      <c r="AV15" s="37">
         <v>224</v>
       </c>
-      <c r="AW15" s="44">
+      <c r="AW15" s="37">
         <v>87</v>
       </c>
-      <c r="AX15" s="45">
+      <c r="AX15" s="38">
         <v>137</v>
       </c>
-      <c r="AY15" s="44">
+      <c r="AY15" s="37">
         <v>253</v>
       </c>
-      <c r="AZ15" s="44">
+      <c r="AZ15" s="37">
         <v>70</v>
       </c>
-      <c r="BA15" s="45">
+      <c r="BA15" s="38">
         <v>183</v>
       </c>
-      <c r="BB15" s="44">
+      <c r="BB15" s="37">
         <v>256</v>
       </c>
-      <c r="BC15" s="44">
+      <c r="BC15" s="37">
         <v>73</v>
       </c>
-      <c r="BD15" s="45">
+      <c r="BD15" s="38">
         <v>183</v>
       </c>
-      <c r="BE15" s="44">
+      <c r="BE15" s="37">
         <v>319</v>
       </c>
-      <c r="BF15" s="44">
+      <c r="BF15" s="37">
         <v>253</v>
       </c>
-      <c r="BG15" s="45">
+      <c r="BG15" s="38">
         <v>66</v>
       </c>
-      <c r="BH15" s="44">
+      <c r="BH15" s="37">
         <v>356</v>
       </c>
-      <c r="BI15" s="44">
+      <c r="BI15" s="37">
         <v>313</v>
       </c>
-      <c r="BJ15" s="45">
+      <c r="BJ15" s="38">
         <v>43</v>
       </c>
     </row>
@@ -3340,94 +3371,94 @@
       <c r="AF16" s="27">
         <v>956</v>
       </c>
-      <c r="AG16" s="44">
+      <c r="AG16" s="37">
         <v>20017</v>
       </c>
-      <c r="AH16" s="44">
+      <c r="AH16" s="37">
         <v>8412</v>
       </c>
-      <c r="AI16" s="45">
+      <c r="AI16" s="38">
         <v>11605</v>
       </c>
-      <c r="AJ16" s="44">
+      <c r="AJ16" s="37">
         <v>17945</v>
       </c>
-      <c r="AK16" s="44">
+      <c r="AK16" s="37">
         <v>8545</v>
       </c>
-      <c r="AL16" s="45">
+      <c r="AL16" s="38">
         <v>9400</v>
       </c>
-      <c r="AM16" s="44">
+      <c r="AM16" s="37">
         <v>18910</v>
       </c>
-      <c r="AN16" s="44">
+      <c r="AN16" s="37">
         <v>8670</v>
       </c>
-      <c r="AO16" s="45">
+      <c r="AO16" s="38">
         <v>10240</v>
       </c>
-      <c r="AP16" s="44">
+      <c r="AP16" s="37">
         <v>21130</v>
       </c>
-      <c r="AQ16" s="44">
+      <c r="AQ16" s="37">
         <v>9472</v>
       </c>
-      <c r="AR16" s="45">
+      <c r="AR16" s="38">
         <v>11658</v>
       </c>
-      <c r="AS16" s="44">
+      <c r="AS16" s="37">
         <v>26671</v>
       </c>
-      <c r="AT16" s="44">
+      <c r="AT16" s="37">
         <v>8952</v>
       </c>
-      <c r="AU16" s="45">
+      <c r="AU16" s="38">
         <v>17719</v>
       </c>
-      <c r="AV16" s="44">
+      <c r="AV16" s="37">
         <v>21899</v>
       </c>
-      <c r="AW16" s="44">
+      <c r="AW16" s="37">
         <v>7221</v>
       </c>
-      <c r="AX16" s="45">
+      <c r="AX16" s="38">
         <v>14678</v>
       </c>
-      <c r="AY16" s="44">
+      <c r="AY16" s="37">
         <v>20264</v>
       </c>
-      <c r="AZ16" s="44">
+      <c r="AZ16" s="37">
         <v>6719</v>
       </c>
-      <c r="BA16" s="45">
+      <c r="BA16" s="38">
         <v>13545</v>
       </c>
-      <c r="BB16" s="44">
+      <c r="BB16" s="37">
         <v>18448</v>
       </c>
-      <c r="BC16" s="44">
+      <c r="BC16" s="37">
         <v>6489</v>
       </c>
-      <c r="BD16" s="45">
+      <c r="BD16" s="38">
         <v>11959</v>
       </c>
-      <c r="BE16" s="44">
+      <c r="BE16" s="37">
         <v>14877</v>
       </c>
-      <c r="BF16" s="44">
+      <c r="BF16" s="37">
         <v>7003</v>
       </c>
-      <c r="BG16" s="45">
+      <c r="BG16" s="38">
         <v>7874</v>
       </c>
-      <c r="BH16" s="44">
+      <c r="BH16" s="37">
         <v>18190</v>
       </c>
-      <c r="BI16" s="44">
+      <c r="BI16" s="37">
         <v>8802</v>
       </c>
-      <c r="BJ16" s="45">
+      <c r="BJ16" s="38">
         <v>9388</v>
       </c>
     </row>
@@ -3528,94 +3559,94 @@
       <c r="AF17" s="27">
         <v>1718</v>
       </c>
-      <c r="AG17" s="44">
+      <c r="AG17" s="37">
         <v>29403</v>
       </c>
-      <c r="AH17" s="44">
+      <c r="AH17" s="37">
         <v>9422</v>
       </c>
-      <c r="AI17" s="45">
+      <c r="AI17" s="38">
         <v>19981</v>
       </c>
-      <c r="AJ17" s="44">
+      <c r="AJ17" s="37">
         <v>30871</v>
       </c>
-      <c r="AK17" s="44">
+      <c r="AK17" s="37">
         <v>11750</v>
       </c>
-      <c r="AL17" s="45">
+      <c r="AL17" s="38">
         <v>19121</v>
       </c>
-      <c r="AM17" s="44">
+      <c r="AM17" s="37">
         <v>38885</v>
       </c>
-      <c r="AN17" s="44">
+      <c r="AN17" s="37">
         <v>13497</v>
       </c>
-      <c r="AO17" s="45">
+      <c r="AO17" s="38">
         <v>25388</v>
       </c>
-      <c r="AP17" s="44">
+      <c r="AP17" s="37">
         <v>47013</v>
       </c>
-      <c r="AQ17" s="44">
+      <c r="AQ17" s="37">
         <v>15426</v>
       </c>
-      <c r="AR17" s="45">
+      <c r="AR17" s="38">
         <v>31587</v>
       </c>
-      <c r="AS17" s="44">
+      <c r="AS17" s="37">
         <v>54405</v>
       </c>
-      <c r="AT17" s="44">
+      <c r="AT17" s="37">
         <v>13722</v>
       </c>
-      <c r="AU17" s="45">
+      <c r="AU17" s="38">
         <v>40683</v>
       </c>
-      <c r="AV17" s="44">
+      <c r="AV17" s="37">
         <v>33379</v>
       </c>
-      <c r="AW17" s="44">
+      <c r="AW17" s="37">
         <v>10509</v>
       </c>
-      <c r="AX17" s="45">
+      <c r="AX17" s="38">
         <v>22870</v>
       </c>
-      <c r="AY17" s="44">
+      <c r="AY17" s="37">
         <v>33886</v>
       </c>
-      <c r="AZ17" s="44">
+      <c r="AZ17" s="37">
         <v>10601</v>
       </c>
-      <c r="BA17" s="45">
+      <c r="BA17" s="38">
         <v>23285</v>
       </c>
-      <c r="BB17" s="44">
+      <c r="BB17" s="37">
         <v>33049</v>
       </c>
-      <c r="BC17" s="44">
+      <c r="BC17" s="37">
         <v>11110</v>
       </c>
-      <c r="BD17" s="45">
+      <c r="BD17" s="38">
         <v>21939</v>
       </c>
-      <c r="BE17" s="44">
+      <c r="BE17" s="37">
         <v>49135</v>
       </c>
-      <c r="BF17" s="44">
+      <c r="BF17" s="37">
         <v>19814</v>
       </c>
-      <c r="BG17" s="45">
+      <c r="BG17" s="38">
         <v>29321</v>
       </c>
-      <c r="BH17" s="44">
+      <c r="BH17" s="37">
         <v>53180</v>
       </c>
-      <c r="BI17" s="44">
+      <c r="BI17" s="37">
         <v>23005</v>
       </c>
-      <c r="BJ17" s="45">
+      <c r="BJ17" s="38">
         <v>30175</v>
       </c>
     </row>
@@ -3716,94 +3747,94 @@
       <c r="AF18" s="27">
         <v>1298</v>
       </c>
-      <c r="AG18" s="44">
+      <c r="AG18" s="37">
         <v>24652</v>
       </c>
-      <c r="AH18" s="44">
+      <c r="AH18" s="37">
         <v>10416</v>
       </c>
-      <c r="AI18" s="45">
+      <c r="AI18" s="38">
         <v>14236</v>
       </c>
-      <c r="AJ18" s="44">
+      <c r="AJ18" s="37">
         <v>22675</v>
       </c>
-      <c r="AK18" s="44">
+      <c r="AK18" s="37">
         <v>10883</v>
       </c>
-      <c r="AL18" s="45">
+      <c r="AL18" s="38">
         <v>11792</v>
       </c>
-      <c r="AM18" s="44">
+      <c r="AM18" s="37">
         <v>31724</v>
       </c>
-      <c r="AN18" s="44">
+      <c r="AN18" s="37">
         <v>13824</v>
       </c>
-      <c r="AO18" s="45">
+      <c r="AO18" s="38">
         <v>17900</v>
       </c>
-      <c r="AP18" s="44">
+      <c r="AP18" s="37">
         <v>36635</v>
       </c>
-      <c r="AQ18" s="44">
+      <c r="AQ18" s="37">
         <v>16598</v>
       </c>
-      <c r="AR18" s="45">
+      <c r="AR18" s="38">
         <v>20037</v>
       </c>
-      <c r="AS18" s="44">
+      <c r="AS18" s="37">
         <v>40877</v>
       </c>
-      <c r="AT18" s="44">
+      <c r="AT18" s="37">
         <v>14064</v>
       </c>
-      <c r="AU18" s="45">
+      <c r="AU18" s="38">
         <v>26813</v>
       </c>
-      <c r="AV18" s="44">
+      <c r="AV18" s="37">
         <v>20298</v>
       </c>
-      <c r="AW18" s="44">
+      <c r="AW18" s="37">
         <v>8556</v>
       </c>
-      <c r="AX18" s="45">
+      <c r="AX18" s="38">
         <v>11742</v>
       </c>
-      <c r="AY18" s="44">
+      <c r="AY18" s="37">
         <v>22015</v>
       </c>
-      <c r="AZ18" s="44">
+      <c r="AZ18" s="37">
         <v>8592</v>
       </c>
-      <c r="BA18" s="45">
+      <c r="BA18" s="38">
         <v>13423</v>
       </c>
-      <c r="BB18" s="44">
+      <c r="BB18" s="37">
         <v>22163</v>
       </c>
-      <c r="BC18" s="44">
+      <c r="BC18" s="37">
         <v>9282</v>
       </c>
-      <c r="BD18" s="45">
+      <c r="BD18" s="38">
         <v>12881</v>
       </c>
-      <c r="BE18" s="44">
+      <c r="BE18" s="37">
         <v>28451</v>
       </c>
-      <c r="BF18" s="44">
+      <c r="BF18" s="37">
         <v>12734</v>
       </c>
-      <c r="BG18" s="45">
+      <c r="BG18" s="38">
         <v>15717</v>
       </c>
-      <c r="BH18" s="44">
+      <c r="BH18" s="37">
         <v>40751</v>
       </c>
-      <c r="BI18" s="44">
+      <c r="BI18" s="37">
         <v>17941</v>
       </c>
-      <c r="BJ18" s="45">
+      <c r="BJ18" s="38">
         <v>22810</v>
       </c>
     </row>
@@ -3904,289 +3935,472 @@
       <c r="AF19" s="27">
         <v>465205</v>
       </c>
-      <c r="AG19" s="44">
+      <c r="AG19" s="37">
         <v>275560</v>
       </c>
-      <c r="AH19" s="44">
+      <c r="AH19" s="37">
         <v>129661</v>
       </c>
-      <c r="AI19" s="45">
+      <c r="AI19" s="38">
         <v>145899</v>
       </c>
-      <c r="AJ19" s="44">
+      <c r="AJ19" s="37">
         <v>287462</v>
       </c>
-      <c r="AK19" s="44">
+      <c r="AK19" s="37">
         <v>145539</v>
       </c>
-      <c r="AL19" s="45">
+      <c r="AL19" s="38">
         <v>141923</v>
       </c>
-      <c r="AM19" s="44">
+      <c r="AM19" s="37">
         <v>300496</v>
       </c>
-      <c r="AN19" s="44">
+      <c r="AN19" s="37">
         <v>151337</v>
       </c>
-      <c r="AO19" s="45">
+      <c r="AO19" s="38">
         <v>149159</v>
       </c>
-      <c r="AP19" s="44">
+      <c r="AP19" s="37">
         <v>306902</v>
       </c>
-      <c r="AQ19" s="44">
+      <c r="AQ19" s="37">
         <v>146170</v>
       </c>
-      <c r="AR19" s="45">
+      <c r="AR19" s="38">
         <v>160732</v>
       </c>
-      <c r="AS19" s="44">
+      <c r="AS19" s="37">
         <v>265086</v>
       </c>
-      <c r="AT19" s="44">
+      <c r="AT19" s="37">
         <v>123202</v>
       </c>
-      <c r="AU19" s="45">
+      <c r="AU19" s="38">
         <v>141884</v>
       </c>
-      <c r="AV19" s="44">
+      <c r="AV19" s="37">
         <v>233222</v>
       </c>
-      <c r="AW19" s="44">
+      <c r="AW19" s="37">
         <v>86771</v>
       </c>
-      <c r="AX19" s="45">
+      <c r="AX19" s="38">
         <v>146451</v>
       </c>
-      <c r="AY19" s="44">
+      <c r="AY19" s="37">
         <v>236205</v>
       </c>
-      <c r="AZ19" s="44">
+      <c r="AZ19" s="37">
         <v>81751</v>
       </c>
-      <c r="BA19" s="45">
+      <c r="BA19" s="38">
         <v>154454</v>
       </c>
-      <c r="BB19" s="44">
+      <c r="BB19" s="37">
         <v>184106</v>
       </c>
-      <c r="BC19" s="44">
+      <c r="BC19" s="37">
         <v>74202</v>
       </c>
-      <c r="BD19" s="45">
+      <c r="BD19" s="38">
         <v>109904</v>
       </c>
-      <c r="BE19" s="44">
+      <c r="BE19" s="37">
         <v>209334</v>
       </c>
-      <c r="BF19" s="44">
+      <c r="BF19" s="37">
         <v>90403</v>
       </c>
-      <c r="BG19" s="45">
+      <c r="BG19" s="38">
         <v>118931</v>
       </c>
-      <c r="BH19" s="44">
+      <c r="BH19" s="37">
         <v>215205</v>
       </c>
-      <c r="BI19" s="44">
+      <c r="BI19" s="37">
         <v>84350</v>
       </c>
-      <c r="BJ19" s="45">
+      <c r="BJ19" s="38">
         <v>130855</v>
       </c>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="52">
+        <v>444</v>
+      </c>
+      <c r="C20" s="53">
+        <v>259</v>
+      </c>
+      <c r="D20" s="54">
+        <v>185</v>
+      </c>
+      <c r="E20" s="52">
+        <v>513</v>
+      </c>
+      <c r="F20" s="53">
+        <v>263</v>
+      </c>
+      <c r="G20" s="54">
+        <v>250</v>
+      </c>
+      <c r="H20" s="52">
+        <v>526</v>
+      </c>
+      <c r="I20" s="53">
+        <v>256</v>
+      </c>
+      <c r="J20" s="54">
+        <v>270</v>
+      </c>
+      <c r="K20" s="52">
+        <v>468</v>
+      </c>
+      <c r="L20" s="53">
+        <v>250</v>
+      </c>
+      <c r="M20" s="54">
+        <v>218</v>
+      </c>
+      <c r="N20" s="52">
+        <v>820</v>
+      </c>
+      <c r="O20" s="53">
+        <v>324</v>
+      </c>
+      <c r="P20" s="54">
+        <v>496</v>
+      </c>
+      <c r="Q20" s="52">
+        <v>947</v>
+      </c>
+      <c r="R20" s="53">
+        <v>410</v>
+      </c>
+      <c r="S20" s="54">
+        <v>537</v>
+      </c>
+      <c r="T20" s="52">
+        <v>1292</v>
+      </c>
+      <c r="U20" s="53">
+        <v>357</v>
+      </c>
+      <c r="V20" s="54">
+        <v>935</v>
+      </c>
+      <c r="W20" s="52">
+        <v>2446</v>
+      </c>
+      <c r="X20" s="53">
+        <v>593</v>
+      </c>
+      <c r="Y20" s="54">
+        <v>1853</v>
+      </c>
+      <c r="Z20" s="52">
+        <v>2307</v>
+      </c>
+      <c r="AA20" s="53">
+        <v>498</v>
+      </c>
+      <c r="AB20" s="54">
+        <v>1809</v>
+      </c>
+      <c r="AC20" s="52">
+        <v>2250</v>
+      </c>
+      <c r="AD20" s="53">
+        <v>495</v>
+      </c>
+      <c r="AE20" s="54">
+        <v>1755</v>
+      </c>
+      <c r="AF20" s="50">
+        <v>167</v>
+      </c>
+      <c r="AG20" s="48">
+        <v>1868</v>
+      </c>
+      <c r="AH20" s="48">
+        <v>805</v>
+      </c>
+      <c r="AI20" s="49">
+        <v>1063</v>
+      </c>
+      <c r="AJ20" s="48">
+        <v>1571</v>
+      </c>
+      <c r="AK20" s="48">
+        <v>712</v>
+      </c>
+      <c r="AL20" s="49">
+        <v>859</v>
+      </c>
+      <c r="AM20" s="48">
+        <v>1426</v>
+      </c>
+      <c r="AN20" s="48">
+        <v>729</v>
+      </c>
+      <c r="AO20" s="49">
+        <v>697</v>
+      </c>
+      <c r="AP20" s="48">
+        <v>1339</v>
+      </c>
+      <c r="AQ20" s="48">
+        <v>692</v>
+      </c>
+      <c r="AR20" s="49">
+        <v>647</v>
+      </c>
+      <c r="AS20" s="48">
+        <v>1318</v>
+      </c>
+      <c r="AT20" s="48">
+        <v>643</v>
+      </c>
+      <c r="AU20" s="49">
+        <v>675</v>
+      </c>
+      <c r="AV20" s="48">
+        <v>930</v>
+      </c>
+      <c r="AW20" s="48">
+        <v>440</v>
+      </c>
+      <c r="AX20" s="49">
+        <v>490</v>
+      </c>
+      <c r="AY20" s="48">
+        <v>882</v>
+      </c>
+      <c r="AZ20" s="48">
+        <v>392</v>
+      </c>
+      <c r="BA20" s="49">
+        <v>490</v>
+      </c>
+      <c r="BB20" s="48">
+        <v>906</v>
+      </c>
+      <c r="BC20" s="48">
+        <v>379</v>
+      </c>
+      <c r="BD20" s="49">
+        <v>527</v>
+      </c>
+      <c r="BE20" s="48">
+        <v>964</v>
+      </c>
+      <c r="BF20" s="48">
+        <v>568</v>
+      </c>
+      <c r="BG20" s="49">
+        <v>396</v>
+      </c>
+      <c r="BH20" s="48">
+        <v>2268</v>
+      </c>
+      <c r="BI20" s="48">
+        <v>1058</v>
+      </c>
+      <c r="BJ20" s="49">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B21" s="9">
         <v>169</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C21" s="10">
         <v>130</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D21" s="11">
         <v>39</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E21" s="9">
         <v>154</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F21" s="10">
         <v>110</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G21" s="11">
         <v>44</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H21" s="9">
         <v>157</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I21" s="10">
         <v>109</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J21" s="11">
         <v>48</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K21" s="9">
         <v>163</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L21" s="10">
         <v>109</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M21" s="11">
         <v>54</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N21" s="9">
         <v>162</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O21" s="10">
         <v>102</v>
       </c>
-      <c r="P20" s="11">
+      <c r="P21" s="11">
         <v>60</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="Q21" s="9">
         <v>188</v>
       </c>
-      <c r="R20" s="10">
+      <c r="R21" s="10">
         <v>128</v>
       </c>
-      <c r="S20" s="11">
+      <c r="S21" s="11">
         <v>60</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T21" s="9">
         <v>187</v>
       </c>
-      <c r="U20" s="10">
+      <c r="U21" s="10">
         <v>124</v>
       </c>
-      <c r="V20" s="11">
+      <c r="V21" s="11">
         <v>63</v>
       </c>
-      <c r="W20" s="9">
+      <c r="W21" s="9">
         <v>209</v>
       </c>
-      <c r="X20" s="10">
+      <c r="X21" s="10">
         <v>117</v>
       </c>
-      <c r="Y20" s="11">
+      <c r="Y21" s="11">
         <v>92</v>
       </c>
-      <c r="Z20" s="9">
+      <c r="Z21" s="9">
         <v>185</v>
       </c>
-      <c r="AA20" s="10">
+      <c r="AA21" s="10">
         <v>102</v>
       </c>
-      <c r="AB20" s="11">
+      <c r="AB21" s="11">
         <v>83</v>
       </c>
-      <c r="AC20" s="9">
+      <c r="AC21" s="9">
         <v>192</v>
       </c>
-      <c r="AD20" s="10">
+      <c r="AD21" s="10">
         <v>100</v>
       </c>
-      <c r="AE20" s="11">
+      <c r="AE21" s="11">
         <v>92</v>
       </c>
-      <c r="AF20" s="27">
+      <c r="AF21" s="27">
         <v>116</v>
       </c>
-      <c r="AG20" s="44">
+      <c r="AG21" s="37">
         <v>190</v>
       </c>
-      <c r="AH20" s="44">
+      <c r="AH21" s="37">
         <v>124</v>
       </c>
-      <c r="AI20" s="45">
+      <c r="AI21" s="38">
         <v>66</v>
       </c>
-      <c r="AJ20" s="44">
+      <c r="AJ21" s="37">
         <v>148</v>
       </c>
-      <c r="AK20" s="44">
+      <c r="AK21" s="37">
         <v>96</v>
       </c>
-      <c r="AL20" s="45">
+      <c r="AL21" s="38">
         <v>52</v>
       </c>
-      <c r="AM20" s="44">
+      <c r="AM21" s="37">
         <v>129</v>
       </c>
-      <c r="AN20" s="44">
+      <c r="AN21" s="37">
         <v>94</v>
       </c>
-      <c r="AO20" s="45">
+      <c r="AO21" s="38">
         <v>35</v>
       </c>
-      <c r="AP20" s="44">
+      <c r="AP21" s="37">
         <v>122</v>
       </c>
-      <c r="AQ20" s="44">
+      <c r="AQ21" s="37">
         <v>82</v>
       </c>
-      <c r="AR20" s="45">
+      <c r="AR21" s="38">
         <v>40</v>
       </c>
-      <c r="AS20" s="44">
+      <c r="AS21" s="37">
         <v>91</v>
       </c>
-      <c r="AT20" s="44">
+      <c r="AT21" s="37">
         <v>56</v>
       </c>
-      <c r="AU20" s="45">
+      <c r="AU21" s="38">
         <v>35</v>
       </c>
-      <c r="AV20" s="44">
+      <c r="AV21" s="37">
         <v>102</v>
       </c>
-      <c r="AW20" s="44">
+      <c r="AW21" s="37">
         <v>57</v>
       </c>
-      <c r="AX20" s="45">
+      <c r="AX21" s="38">
         <v>45</v>
       </c>
-      <c r="AY20" s="44">
+      <c r="AY21" s="37">
         <v>83</v>
       </c>
-      <c r="AZ20" s="44">
+      <c r="AZ21" s="37">
         <v>54</v>
       </c>
-      <c r="BA20" s="45">
+      <c r="BA21" s="38">
         <v>29</v>
       </c>
-      <c r="BB20" s="44">
+      <c r="BB21" s="37">
         <v>94</v>
       </c>
-      <c r="BC20" s="44">
+      <c r="BC21" s="37">
         <v>52</v>
       </c>
-      <c r="BD20" s="45">
+      <c r="BD21" s="38">
         <v>42</v>
       </c>
-      <c r="BE20" s="44">
+      <c r="BE21" s="37">
         <v>91</v>
       </c>
-      <c r="BF20" s="44">
+      <c r="BF21" s="37">
         <v>86</v>
       </c>
-      <c r="BG20" s="45">
+      <c r="BG21" s="38">
         <v>5</v>
       </c>
-      <c r="BH20" s="44">
+      <c r="BH21" s="37">
         <v>102</v>
       </c>
-      <c r="BI20" s="44">
+      <c r="BI21" s="37">
         <v>95</v>
       </c>
-      <c r="BJ20" s="45">
+      <c r="BJ21" s="38">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="AC21"/>
-      <c r="AD21"/>
-      <c r="AE21"/>
     </row>
     <row r="22" spans="1:62" x14ac:dyDescent="0.25">
       <c r="AC22"/>
@@ -4444,53 +4658,58 @@
       <c r="AE72"/>
     </row>
     <row r="73" spans="8:31" x14ac:dyDescent="0.25">
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="5"/>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
-      <c r="U73" s="5"/>
-      <c r="V73" s="5"/>
-      <c r="W73" s="5"/>
-      <c r="X73" s="5"/>
-      <c r="Y73" s="5"/>
-      <c r="Z73" s="5"/>
-      <c r="AA73" s="5"/>
-      <c r="AB73" s="5"/>
-    </row>
-    <row r="80" spans="8:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AC73"/>
+      <c r="AD73"/>
+      <c r="AE73"/>
+    </row>
+    <row r="74" spans="8:31" x14ac:dyDescent="0.25">
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
+      <c r="U74" s="5"/>
+      <c r="V74" s="5"/>
+      <c r="W74" s="5"/>
+      <c r="X74" s="5"/>
+      <c r="Y74" s="5"/>
+      <c r="Z74" s="5"/>
+      <c r="AA74" s="5"/>
+      <c r="AB74" s="5"/>
+    </row>
+    <row r="81" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="AV1:AX1"/>
+    <mergeCell ref="AY1:BA1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="BE1:BG1"/>
+    <mergeCell ref="BH1:BJ1"/>
     <mergeCell ref="AG1:AI1"/>
     <mergeCell ref="AJ1:AL1"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="AP1:AR1"/>
     <mergeCell ref="AS1:AU1"/>
-    <mergeCell ref="AV1:AX1"/>
-    <mergeCell ref="AY1:BA1"/>
-    <mergeCell ref="BB1:BD1"/>
-    <mergeCell ref="BE1:BG1"/>
-    <mergeCell ref="BH1:BJ1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
basic pandas and plotly viz of enf data, data format change in t41
</commit_message>
<xml_diff>
--- a/data/t41_2000-2019.xlsx
+++ b/data/t41_2000-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\watti\OneDrive\Desktop\mit\11.154 datasets\11.154-proj-pathways\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788C09BC-E359-4E42-9F94-011730982DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC594798-4944-4B70-8267-B6B6CF2F8285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13920" yWindow="2370" windowWidth="11400" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table removals37" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="16">
   <si>
     <t xml:space="preserve">Region and country of nationality  </t>
   </si>
@@ -69,36 +69,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
     <r>
       <t>Criminal</t>
     </r>
@@ -119,6 +89,9 @@
   <si>
     <t>Global Total</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -128,7 +101,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -164,6 +137,11 @@
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -305,7 +283,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -318,7 +296,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -362,9 +339,6 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -385,27 +359,32 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -726,9 +705,9 @@
   <dimension ref="A1:BJ71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
       <selection activeCell="A143" sqref="A143"/>
-      <selection pane="topRight" activeCell="H6" sqref="H6"/>
+      <selection pane="topRight" activeCell="AM16" sqref="AM16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -736,119 +715,121 @@
     <col min="1" max="1" width="33.5546875" customWidth="1"/>
     <col min="2" max="4" width="9.44140625" customWidth="1"/>
     <col min="5" max="28" width="9" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="33">
+    <row r="1" spans="1:62" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="32">
         <v>1999</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32">
         <v>2000</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33">
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32">
         <v>2001</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32">
         <v>2002</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33">
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32">
         <v>2003</v>
       </c>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33">
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32">
         <v>2004</v>
       </c>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33">
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32">
         <v>2005</v>
       </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
       <c r="W1" s="33">
         <v>2006</v>
       </c>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33">
+      <c r="X1" s="34"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="32">
         <v>2007</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="34">
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="33">
         <v>2008</v>
       </c>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="24">
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="36">
         <v>2009</v>
       </c>
-      <c r="AG1" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="39"/>
-      <c r="AP1" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="39"/>
-      <c r="AS1" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="39"/>
-      <c r="AV1" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="39"/>
-      <c r="AY1" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="AZ1" s="38"/>
-      <c r="BA1" s="39"/>
-      <c r="BB1" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="BC1" s="38"/>
-      <c r="BD1" s="39"/>
-      <c r="BE1" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="BF1" s="38"/>
-      <c r="BG1" s="39"/>
-      <c r="BH1" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="BI1" s="38"/>
-      <c r="BJ1" s="39"/>
+      <c r="AG1" s="31">
+        <v>2010</v>
+      </c>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="31">
+        <v>2011</v>
+      </c>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="31">
+        <v>2012</v>
+      </c>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="31">
+        <v>2013</v>
+      </c>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="31">
+        <v>2014</v>
+      </c>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="31">
+        <v>2015</v>
+      </c>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="38"/>
+      <c r="AY1" s="31">
+        <v>2016</v>
+      </c>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="37">
+        <v>2017</v>
+      </c>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="38"/>
+      <c r="BE1" s="31">
+        <v>2018</v>
+      </c>
+      <c r="BF1" s="37"/>
+      <c r="BG1" s="38"/>
+      <c r="BH1" s="31">
+        <v>2019</v>
+      </c>
+      <c r="BI1" s="37"/>
+      <c r="BJ1" s="38"/>
     </row>
     <row r="2" spans="1:62" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -932,294 +913,294 @@
       <c r="AB2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AD2" s="13" t="s">
+      <c r="AD2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="AE2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AF2" s="25" t="s">
+      <c r="AF2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="AG2" s="17" t="s">
+      <c r="AG2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AH2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI2" s="19" t="s">
+      <c r="AH2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AJ2" s="18" t="s">
+      <c r="AJ2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AK2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL2" s="18" t="s">
+      <c r="AK2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="AM2" s="17" t="s">
+      <c r="AM2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AN2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO2" s="19" t="s">
+      <c r="AN2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AP2" s="18" t="s">
+      <c r="AP2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR2" s="18" t="s">
+      <c r="AQ2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="AS2" s="17" t="s">
+      <c r="AS2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU2" s="19" t="s">
+      <c r="AT2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AV2" s="18" t="s">
+      <c r="AV2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AW2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX2" s="18" t="s">
+      <c r="AW2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="17" t="s">
+      <c r="AY2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="AZ2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA2" s="19" t="s">
+      <c r="AZ2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="BB2" s="18" t="s">
+      <c r="BB2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="BC2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD2" s="19" t="s">
+      <c r="BC2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="BD2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="BE2" s="17" t="s">
+      <c r="BE2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="BF2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="BG2" s="19" t="s">
+      <c r="BF2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="BG2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="BH2" s="17" t="s">
+      <c r="BH2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="BI2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="BJ2" s="19" t="s">
+      <c r="BI2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ2" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6">
         <v>183114</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>71188</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>111926</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>188467</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>73065</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>115402</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>189026</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>73545</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>115481</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>165168</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>72818</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="8">
         <v>92350</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="6">
         <v>211098</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <v>82822</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="8">
         <v>128276</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="6">
         <v>240665</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3" s="7">
         <v>91508</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="8">
         <v>149157</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="6">
         <v>246431</v>
       </c>
-      <c r="U3" s="8">
+      <c r="U3" s="7">
         <v>91725</v>
       </c>
-      <c r="V3" s="9">
+      <c r="V3" s="8">
         <v>154706</v>
       </c>
-      <c r="W3" s="7">
+      <c r="W3" s="6">
         <v>280974</v>
       </c>
-      <c r="X3" s="8">
+      <c r="X3" s="7">
         <v>97365</v>
       </c>
-      <c r="Y3" s="9">
+      <c r="Y3" s="8">
         <v>183609</v>
       </c>
-      <c r="Z3" s="7">
+      <c r="Z3" s="6">
         <v>319382</v>
       </c>
-      <c r="AA3" s="8">
+      <c r="AA3" s="7">
         <v>99924</v>
       </c>
-      <c r="AB3" s="9">
+      <c r="AB3" s="8">
         <v>219458</v>
       </c>
-      <c r="AC3" s="7">
+      <c r="AC3" s="6">
         <v>358886</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AD3" s="7">
         <v>97133</v>
       </c>
-      <c r="AE3" s="9">
+      <c r="AE3" s="8">
         <v>261753</v>
       </c>
-      <c r="AF3" s="16">
+      <c r="AF3" s="15">
         <v>580107</v>
       </c>
-      <c r="AG3" s="20">
+      <c r="AG3" s="19">
         <v>382449</v>
       </c>
-      <c r="AH3" s="20">
+      <c r="AH3" s="19">
         <v>171030</v>
       </c>
-      <c r="AI3" s="21">
+      <c r="AI3" s="20">
         <v>211419</v>
       </c>
-      <c r="AJ3" s="20">
+      <c r="AJ3" s="19">
         <v>390423</v>
       </c>
-      <c r="AK3" s="20">
+      <c r="AK3" s="19">
         <v>189702</v>
       </c>
-      <c r="AL3" s="21">
+      <c r="AL3" s="20">
         <v>200721</v>
       </c>
-      <c r="AM3" s="20">
+      <c r="AM3" s="19">
         <v>415607</v>
       </c>
-      <c r="AN3" s="20">
+      <c r="AN3" s="19">
         <v>200039</v>
       </c>
-      <c r="AO3" s="21">
+      <c r="AO3" s="20">
         <v>215568</v>
       </c>
-      <c r="AP3" s="20">
+      <c r="AP3" s="19">
         <v>432228</v>
       </c>
-      <c r="AQ3" s="20">
+      <c r="AQ3" s="19">
         <v>198488</v>
       </c>
-      <c r="AR3" s="21">
+      <c r="AR3" s="20">
         <v>233740</v>
       </c>
-      <c r="AS3" s="20">
+      <c r="AS3" s="19">
         <v>405090</v>
       </c>
-      <c r="AT3" s="20">
+      <c r="AT3" s="19">
         <v>169459</v>
       </c>
-      <c r="AU3" s="21">
+      <c r="AU3" s="20">
         <v>235631</v>
       </c>
-      <c r="AV3" s="20">
+      <c r="AV3" s="19">
         <v>325328</v>
       </c>
-      <c r="AW3" s="20">
+      <c r="AW3" s="19">
         <v>120846</v>
       </c>
-      <c r="AX3" s="21">
+      <c r="AX3" s="20">
         <v>204482</v>
       </c>
-      <c r="AY3" s="20">
+      <c r="AY3" s="19">
         <v>331717</v>
       </c>
-      <c r="AZ3" s="20">
+      <c r="AZ3" s="19">
         <v>115301</v>
       </c>
-      <c r="BA3" s="21">
+      <c r="BA3" s="20">
         <v>216416</v>
       </c>
-      <c r="BB3" s="20">
+      <c r="BB3" s="19">
         <v>287093</v>
       </c>
-      <c r="BC3" s="20">
+      <c r="BC3" s="19">
         <v>109697</v>
       </c>
-      <c r="BD3" s="21">
+      <c r="BD3" s="20">
         <v>177396</v>
       </c>
-      <c r="BE3" s="20">
+      <c r="BE3" s="19">
         <v>328716</v>
       </c>
-      <c r="BF3" s="20">
+      <c r="BF3" s="19">
         <v>148352</v>
       </c>
-      <c r="BG3" s="21">
+      <c r="BG3" s="20">
         <v>180364</v>
       </c>
-      <c r="BH3" s="20">
+      <c r="BH3" s="19">
         <v>359885</v>
       </c>
-      <c r="BI3" s="20">
+      <c r="BI3" s="19">
         <v>155788</v>
       </c>
-      <c r="BJ3" s="21">
+      <c r="BJ3" s="20">
         <v>204097</v>
       </c>
     </row>
@@ -1227,187 +1208,187 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>191</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>139</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>52</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>170</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>126</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>44</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>185</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>110</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>75</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>178</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
         <v>116</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="8">
         <v>62</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="6">
         <v>179</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>117</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="8">
         <v>62</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="6">
         <v>202</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4" s="7">
         <v>122</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="8">
         <v>80</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="6">
         <v>219</v>
       </c>
-      <c r="U4" s="8">
+      <c r="U4" s="7">
         <v>122</v>
       </c>
-      <c r="V4" s="9">
+      <c r="V4" s="8">
         <v>97</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="6">
         <v>211</v>
       </c>
-      <c r="X4" s="8">
+      <c r="X4" s="7">
         <v>113</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="Y4" s="8">
         <v>98</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="Z4" s="6">
         <v>233</v>
       </c>
-      <c r="AA4" s="8">
+      <c r="AA4" s="7">
         <v>116</v>
       </c>
-      <c r="AB4" s="9">
+      <c r="AB4" s="8">
         <v>117</v>
       </c>
-      <c r="AC4" s="7">
+      <c r="AC4" s="6">
         <v>218</v>
       </c>
-      <c r="AD4" s="8">
+      <c r="AD4" s="7">
         <v>111</v>
       </c>
-      <c r="AE4" s="9">
+      <c r="AE4" s="8">
         <v>107</v>
       </c>
-      <c r="AF4" s="16">
+      <c r="AF4" s="15">
         <v>63</v>
       </c>
-      <c r="AG4" s="22">
+      <c r="AG4" s="21">
         <v>254</v>
       </c>
-      <c r="AH4" s="22">
+      <c r="AH4" s="21">
         <v>157</v>
       </c>
-      <c r="AI4" s="23">
+      <c r="AI4" s="22">
         <v>97</v>
       </c>
-      <c r="AJ4" s="22">
+      <c r="AJ4" s="21">
         <v>221</v>
       </c>
-      <c r="AK4" s="22">
+      <c r="AK4" s="21">
         <v>158</v>
       </c>
-      <c r="AL4" s="23">
+      <c r="AL4" s="22">
         <v>63</v>
       </c>
-      <c r="AM4" s="22">
+      <c r="AM4" s="21">
         <v>204</v>
       </c>
-      <c r="AN4" s="22">
+      <c r="AN4" s="21">
         <v>146</v>
       </c>
-      <c r="AO4" s="23">
+      <c r="AO4" s="22">
         <v>58</v>
       </c>
-      <c r="AP4" s="22">
+      <c r="AP4" s="21">
         <v>175</v>
       </c>
-      <c r="AQ4" s="22">
+      <c r="AQ4" s="21">
         <v>121</v>
       </c>
-      <c r="AR4" s="23">
+      <c r="AR4" s="22">
         <v>54</v>
       </c>
-      <c r="AS4" s="22">
+      <c r="AS4" s="21">
         <v>136</v>
       </c>
-      <c r="AT4" s="22">
+      <c r="AT4" s="21">
         <v>79</v>
       </c>
-      <c r="AU4" s="23">
+      <c r="AU4" s="22">
         <v>57</v>
       </c>
-      <c r="AV4" s="22">
+      <c r="AV4" s="21">
         <v>134</v>
       </c>
-      <c r="AW4" s="22">
+      <c r="AW4" s="21">
         <v>83</v>
       </c>
-      <c r="AX4" s="23">
+      <c r="AX4" s="22">
         <v>51</v>
       </c>
-      <c r="AY4" s="22">
+      <c r="AY4" s="21">
         <v>146</v>
       </c>
-      <c r="AZ4" s="22">
+      <c r="AZ4" s="21">
         <v>86</v>
       </c>
-      <c r="BA4" s="23">
+      <c r="BA4" s="22">
         <v>60</v>
       </c>
-      <c r="BB4" s="22">
+      <c r="BB4" s="21">
         <v>123</v>
       </c>
-      <c r="BC4" s="22">
+      <c r="BC4" s="21">
         <v>57</v>
       </c>
-      <c r="BD4" s="23">
+      <c r="BD4" s="22">
         <v>66</v>
       </c>
-      <c r="BE4" s="22">
+      <c r="BE4" s="21">
         <v>133</v>
       </c>
-      <c r="BF4" s="22">
+      <c r="BF4" s="21">
         <v>111</v>
       </c>
-      <c r="BG4" s="23">
+      <c r="BG4" s="22">
         <v>22</v>
       </c>
-      <c r="BH4" s="22">
+      <c r="BH4" s="21">
         <v>109</v>
       </c>
-      <c r="BI4" s="22">
+      <c r="BI4" s="21">
         <v>80</v>
       </c>
-      <c r="BJ4" s="23">
+      <c r="BJ4" s="22">
         <v>29</v>
       </c>
     </row>
@@ -1415,187 +1396,187 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>227</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>69</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>158</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>328</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>58</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>270</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>392</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>65</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>327</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>376</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="7">
         <v>56</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>320</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <v>514</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="7">
         <v>64</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>450</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="6">
         <v>599</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="7">
         <v>75</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="8">
         <v>524</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="6">
         <v>676</v>
       </c>
-      <c r="U5" s="8">
+      <c r="U5" s="7">
         <v>86</v>
       </c>
-      <c r="V5" s="9">
+      <c r="V5" s="8">
         <v>590</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="6">
         <v>795</v>
       </c>
-      <c r="X5" s="8">
+      <c r="X5" s="7">
         <v>95</v>
       </c>
-      <c r="Y5" s="9">
+      <c r="Y5" s="8">
         <v>700</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="Z5" s="6">
         <v>655</v>
       </c>
-      <c r="AA5" s="8">
+      <c r="AA5" s="7">
         <v>78</v>
       </c>
-      <c r="AB5" s="9">
+      <c r="AB5" s="8">
         <v>577</v>
       </c>
-      <c r="AC5" s="7">
+      <c r="AC5" s="6">
         <v>687</v>
       </c>
-      <c r="AD5" s="8">
+      <c r="AD5" s="7">
         <v>128</v>
       </c>
-      <c r="AE5" s="9">
+      <c r="AE5" s="8">
         <v>559</v>
       </c>
-      <c r="AF5" s="16">
+      <c r="AF5" s="15">
         <v>152</v>
       </c>
-      <c r="AG5" s="22">
+      <c r="AG5" s="21">
         <v>558</v>
       </c>
-      <c r="AH5" s="22">
+      <c r="AH5" s="21">
         <v>159</v>
       </c>
-      <c r="AI5" s="23">
+      <c r="AI5" s="22">
         <v>399</v>
       </c>
-      <c r="AJ5" s="22">
+      <c r="AJ5" s="21">
         <v>415</v>
       </c>
-      <c r="AK5" s="22">
+      <c r="AK5" s="21">
         <v>161</v>
       </c>
-      <c r="AL5" s="23">
+      <c r="AL5" s="22">
         <v>254</v>
       </c>
-      <c r="AM5" s="22">
+      <c r="AM5" s="21">
         <v>398</v>
       </c>
-      <c r="AN5" s="22">
+      <c r="AN5" s="21">
         <v>131</v>
       </c>
-      <c r="AO5" s="23">
+      <c r="AO5" s="22">
         <v>267</v>
       </c>
-      <c r="AP5" s="22">
+      <c r="AP5" s="21">
         <v>332</v>
       </c>
-      <c r="AQ5" s="22">
+      <c r="AQ5" s="21">
         <v>128</v>
       </c>
-      <c r="AR5" s="23">
+      <c r="AR5" s="22">
         <v>204</v>
       </c>
-      <c r="AS5" s="22">
+      <c r="AS5" s="21">
         <v>286</v>
       </c>
-      <c r="AT5" s="22">
+      <c r="AT5" s="21">
         <v>125</v>
       </c>
-      <c r="AU5" s="23">
+      <c r="AU5" s="22">
         <v>161</v>
       </c>
-      <c r="AV5" s="22">
+      <c r="AV5" s="21">
         <v>224</v>
       </c>
-      <c r="AW5" s="22">
+      <c r="AW5" s="21">
         <v>87</v>
       </c>
-      <c r="AX5" s="23">
+      <c r="AX5" s="22">
         <v>137</v>
       </c>
-      <c r="AY5" s="22">
+      <c r="AY5" s="21">
         <v>253</v>
       </c>
-      <c r="AZ5" s="22">
+      <c r="AZ5" s="21">
         <v>70</v>
       </c>
-      <c r="BA5" s="23">
+      <c r="BA5" s="22">
         <v>183</v>
       </c>
-      <c r="BB5" s="22">
+      <c r="BB5" s="21">
         <v>256</v>
       </c>
-      <c r="BC5" s="22">
+      <c r="BC5" s="21">
         <v>73</v>
       </c>
-      <c r="BD5" s="23">
+      <c r="BD5" s="22">
         <v>183</v>
       </c>
-      <c r="BE5" s="22">
+      <c r="BE5" s="21">
         <v>319</v>
       </c>
-      <c r="BF5" s="22">
+      <c r="BF5" s="21">
         <v>253</v>
       </c>
-      <c r="BG5" s="23">
+      <c r="BG5" s="22">
         <v>66</v>
       </c>
-      <c r="BH5" s="22">
+      <c r="BH5" s="21">
         <v>356</v>
       </c>
-      <c r="BI5" s="22">
+      <c r="BI5" s="21">
         <v>313</v>
       </c>
-      <c r="BJ5" s="23">
+      <c r="BJ5" s="22">
         <v>43</v>
       </c>
     </row>
@@ -1603,187 +1584,187 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>4160</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>2115</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>2045</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>4736</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>2145</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>2591</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>3928</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>1895</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>2033</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>4066</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>1771</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="8">
         <v>2295</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="6">
         <v>5561</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>2087</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="8">
         <v>3474</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="6">
         <v>7269</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="7">
         <v>2794</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="8">
         <v>4475</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="6">
         <v>8305</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6" s="7">
         <v>2808</v>
       </c>
-      <c r="V6" s="9">
+      <c r="V6" s="8">
         <v>5497</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="6">
         <v>11050</v>
       </c>
-      <c r="X6" s="8">
+      <c r="X6" s="7">
         <v>3731</v>
       </c>
-      <c r="Y6" s="9">
+      <c r="Y6" s="8">
         <v>7319</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="Z6" s="6">
         <v>20045</v>
       </c>
-      <c r="AA6" s="8">
+      <c r="AA6" s="7">
         <v>4669</v>
       </c>
-      <c r="AB6" s="9">
+      <c r="AB6" s="8">
         <v>15376</v>
       </c>
-      <c r="AC6" s="7">
+      <c r="AC6" s="6">
         <v>20031</v>
       </c>
-      <c r="AD6" s="8">
+      <c r="AD6" s="7">
         <v>4795</v>
       </c>
-      <c r="AE6" s="9">
+      <c r="AE6" s="8">
         <v>15236</v>
       </c>
-      <c r="AF6" s="16">
+      <c r="AF6" s="15">
         <v>956</v>
       </c>
-      <c r="AG6" s="22">
+      <c r="AG6" s="21">
         <v>20017</v>
       </c>
-      <c r="AH6" s="22">
+      <c r="AH6" s="21">
         <v>8412</v>
       </c>
-      <c r="AI6" s="23">
+      <c r="AI6" s="22">
         <v>11605</v>
       </c>
-      <c r="AJ6" s="22">
+      <c r="AJ6" s="21">
         <v>17945</v>
       </c>
-      <c r="AK6" s="22">
+      <c r="AK6" s="21">
         <v>8545</v>
       </c>
-      <c r="AL6" s="23">
+      <c r="AL6" s="22">
         <v>9400</v>
       </c>
-      <c r="AM6" s="22">
+      <c r="AM6" s="21">
         <v>18910</v>
       </c>
-      <c r="AN6" s="22">
+      <c r="AN6" s="21">
         <v>8670</v>
       </c>
-      <c r="AO6" s="23">
+      <c r="AO6" s="22">
         <v>10240</v>
       </c>
-      <c r="AP6" s="22">
+      <c r="AP6" s="21">
         <v>21130</v>
       </c>
-      <c r="AQ6" s="22">
+      <c r="AQ6" s="21">
         <v>9472</v>
       </c>
-      <c r="AR6" s="23">
+      <c r="AR6" s="22">
         <v>11658</v>
       </c>
-      <c r="AS6" s="22">
+      <c r="AS6" s="21">
         <v>26671</v>
       </c>
-      <c r="AT6" s="22">
+      <c r="AT6" s="21">
         <v>8952</v>
       </c>
-      <c r="AU6" s="23">
+      <c r="AU6" s="22">
         <v>17719</v>
       </c>
-      <c r="AV6" s="22">
+      <c r="AV6" s="21">
         <v>21899</v>
       </c>
-      <c r="AW6" s="22">
+      <c r="AW6" s="21">
         <v>7221</v>
       </c>
-      <c r="AX6" s="23">
+      <c r="AX6" s="22">
         <v>14678</v>
       </c>
-      <c r="AY6" s="22">
+      <c r="AY6" s="21">
         <v>20264</v>
       </c>
-      <c r="AZ6" s="22">
+      <c r="AZ6" s="21">
         <v>6719</v>
       </c>
-      <c r="BA6" s="23">
+      <c r="BA6" s="22">
         <v>13545</v>
       </c>
-      <c r="BB6" s="22">
+      <c r="BB6" s="21">
         <v>18448</v>
       </c>
-      <c r="BC6" s="22">
+      <c r="BC6" s="21">
         <v>6489</v>
       </c>
-      <c r="BD6" s="23">
+      <c r="BD6" s="22">
         <v>11959</v>
       </c>
-      <c r="BE6" s="22">
+      <c r="BE6" s="21">
         <v>14877</v>
       </c>
-      <c r="BF6" s="22">
+      <c r="BF6" s="21">
         <v>7003</v>
       </c>
-      <c r="BG6" s="23">
+      <c r="BG6" s="22">
         <v>7874</v>
       </c>
-      <c r="BH6" s="22">
+      <c r="BH6" s="21">
         <v>18190</v>
       </c>
-      <c r="BI6" s="22">
+      <c r="BI6" s="21">
         <v>8802</v>
       </c>
-      <c r="BJ6" s="23">
+      <c r="BJ6" s="22">
         <v>9388</v>
       </c>
     </row>
@@ -1791,187 +1772,187 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>3763</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>1096</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>2667</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>4543</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>1203</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>3340</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>4716</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>1169</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>3547</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>5396</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>1256</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="8">
         <v>4140</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <v>7726</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="7">
         <v>1590</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="8">
         <v>6136</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="6">
         <v>9729</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7" s="7">
         <v>1963</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="8">
         <v>7766</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="6">
         <v>14522</v>
       </c>
-      <c r="U7" s="8">
+      <c r="U7" s="7">
         <v>1935</v>
       </c>
-      <c r="V7" s="9">
+      <c r="V7" s="8">
         <v>12587</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W7" s="6">
         <v>20527</v>
       </c>
-      <c r="X7" s="8">
+      <c r="X7" s="7">
         <v>3649</v>
       </c>
-      <c r="Y7" s="9">
+      <c r="Y7" s="8">
         <v>16878</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="Z7" s="6">
         <v>25898</v>
       </c>
-      <c r="AA7" s="8">
+      <c r="AA7" s="7">
         <v>3477</v>
       </c>
-      <c r="AB7" s="9">
+      <c r="AB7" s="8">
         <v>22421</v>
       </c>
-      <c r="AC7" s="7">
+      <c r="AC7" s="6">
         <v>27594</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AD7" s="7">
         <v>4061</v>
       </c>
-      <c r="AE7" s="9">
+      <c r="AE7" s="8">
         <v>23533</v>
       </c>
-      <c r="AF7" s="16">
+      <c r="AF7" s="15">
         <v>1718</v>
       </c>
-      <c r="AG7" s="22">
+      <c r="AG7" s="21">
         <v>29403</v>
       </c>
-      <c r="AH7" s="22">
+      <c r="AH7" s="21">
         <v>9422</v>
       </c>
-      <c r="AI7" s="23">
+      <c r="AI7" s="22">
         <v>19981</v>
       </c>
-      <c r="AJ7" s="22">
+      <c r="AJ7" s="21">
         <v>30871</v>
       </c>
-      <c r="AK7" s="22">
+      <c r="AK7" s="21">
         <v>11750</v>
       </c>
-      <c r="AL7" s="23">
+      <c r="AL7" s="22">
         <v>19121</v>
       </c>
-      <c r="AM7" s="22">
+      <c r="AM7" s="21">
         <v>38885</v>
       </c>
-      <c r="AN7" s="22">
+      <c r="AN7" s="21">
         <v>13497</v>
       </c>
-      <c r="AO7" s="23">
+      <c r="AO7" s="22">
         <v>25388</v>
       </c>
-      <c r="AP7" s="22">
+      <c r="AP7" s="21">
         <v>47013</v>
       </c>
-      <c r="AQ7" s="22">
+      <c r="AQ7" s="21">
         <v>15426</v>
       </c>
-      <c r="AR7" s="23">
+      <c r="AR7" s="22">
         <v>31587</v>
       </c>
-      <c r="AS7" s="22">
+      <c r="AS7" s="21">
         <v>54405</v>
       </c>
-      <c r="AT7" s="22">
+      <c r="AT7" s="21">
         <v>13722</v>
       </c>
-      <c r="AU7" s="23">
+      <c r="AU7" s="22">
         <v>40683</v>
       </c>
-      <c r="AV7" s="22">
+      <c r="AV7" s="21">
         <v>33379</v>
       </c>
-      <c r="AW7" s="22">
+      <c r="AW7" s="21">
         <v>10509</v>
       </c>
-      <c r="AX7" s="23">
+      <c r="AX7" s="22">
         <v>22870</v>
       </c>
-      <c r="AY7" s="22">
+      <c r="AY7" s="21">
         <v>33886</v>
       </c>
-      <c r="AZ7" s="22">
+      <c r="AZ7" s="21">
         <v>10601</v>
       </c>
-      <c r="BA7" s="23">
+      <c r="BA7" s="22">
         <v>23285</v>
       </c>
-      <c r="BB7" s="22">
+      <c r="BB7" s="21">
         <v>33049</v>
       </c>
-      <c r="BC7" s="22">
+      <c r="BC7" s="21">
         <v>11110</v>
       </c>
-      <c r="BD7" s="23">
+      <c r="BD7" s="22">
         <v>21939</v>
       </c>
-      <c r="BE7" s="22">
+      <c r="BE7" s="21">
         <v>49135</v>
       </c>
-      <c r="BF7" s="22">
+      <c r="BF7" s="21">
         <v>19814</v>
       </c>
-      <c r="BG7" s="23">
+      <c r="BG7" s="22">
         <v>29321</v>
       </c>
-      <c r="BH7" s="22">
+      <c r="BH7" s="21">
         <v>53180</v>
       </c>
-      <c r="BI7" s="22">
+      <c r="BI7" s="21">
         <v>23005</v>
       </c>
-      <c r="BJ7" s="23">
+      <c r="BJ7" s="22">
         <v>30175</v>
       </c>
     </row>
@@ -1979,187 +1960,187 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>3460</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>1255</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>2205</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>4768</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>1486</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>3282</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>4548</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>1429</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="8">
         <v>3119</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>4946</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>1502</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="8">
         <v>3444</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <v>8182</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="7">
         <v>2029</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P8" s="8">
         <v>6153</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="6">
         <v>8752</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8" s="7">
         <v>2517</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="8">
         <v>6235</v>
       </c>
-      <c r="T8" s="7">
+      <c r="T8" s="6">
         <v>15572</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8" s="7">
         <v>2659</v>
       </c>
-      <c r="V8" s="9">
+      <c r="V8" s="8">
         <v>12913</v>
       </c>
-      <c r="W8" s="7">
+      <c r="W8" s="6">
         <v>27060</v>
       </c>
-      <c r="X8" s="8">
+      <c r="X8" s="7">
         <v>5674</v>
       </c>
-      <c r="Y8" s="9">
+      <c r="Y8" s="8">
         <v>21386</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="Z8" s="9">
         <v>29737</v>
       </c>
-      <c r="AA8" s="8">
+      <c r="AA8" s="7">
         <v>5032</v>
       </c>
-      <c r="AB8" s="9">
+      <c r="AB8" s="8">
         <v>24705</v>
       </c>
-      <c r="AC8" s="7">
+      <c r="AC8" s="6">
         <v>28851</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AD8" s="7">
         <v>4944</v>
       </c>
-      <c r="AE8" s="9">
+      <c r="AE8" s="8">
         <v>23907</v>
       </c>
-      <c r="AF8" s="16">
+      <c r="AF8" s="15">
         <v>1298</v>
       </c>
-      <c r="AG8" s="22">
+      <c r="AG8" s="21">
         <v>24652</v>
       </c>
-      <c r="AH8" s="22">
+      <c r="AH8" s="21">
         <v>10416</v>
       </c>
-      <c r="AI8" s="23">
+      <c r="AI8" s="22">
         <v>14236</v>
       </c>
-      <c r="AJ8" s="22">
+      <c r="AJ8" s="21">
         <v>22675</v>
       </c>
-      <c r="AK8" s="22">
+      <c r="AK8" s="21">
         <v>10883</v>
       </c>
-      <c r="AL8" s="23">
+      <c r="AL8" s="22">
         <v>11792</v>
       </c>
-      <c r="AM8" s="22">
+      <c r="AM8" s="21">
         <v>31724</v>
       </c>
-      <c r="AN8" s="22">
+      <c r="AN8" s="21">
         <v>13824</v>
       </c>
-      <c r="AO8" s="23">
+      <c r="AO8" s="22">
         <v>17900</v>
       </c>
-      <c r="AP8" s="22">
+      <c r="AP8" s="21">
         <v>36635</v>
       </c>
-      <c r="AQ8" s="22">
+      <c r="AQ8" s="21">
         <v>16598</v>
       </c>
-      <c r="AR8" s="23">
+      <c r="AR8" s="22">
         <v>20037</v>
       </c>
-      <c r="AS8" s="22">
+      <c r="AS8" s="21">
         <v>40877</v>
       </c>
-      <c r="AT8" s="22">
+      <c r="AT8" s="21">
         <v>14064</v>
       </c>
-      <c r="AU8" s="23">
+      <c r="AU8" s="22">
         <v>26813</v>
       </c>
-      <c r="AV8" s="22">
+      <c r="AV8" s="21">
         <v>20298</v>
       </c>
-      <c r="AW8" s="22">
+      <c r="AW8" s="21">
         <v>8556</v>
       </c>
-      <c r="AX8" s="23">
+      <c r="AX8" s="22">
         <v>11742</v>
       </c>
-      <c r="AY8" s="22">
+      <c r="AY8" s="21">
         <v>22015</v>
       </c>
-      <c r="AZ8" s="22">
+      <c r="AZ8" s="21">
         <v>8592</v>
       </c>
-      <c r="BA8" s="23">
+      <c r="BA8" s="22">
         <v>13423</v>
       </c>
-      <c r="BB8" s="22">
+      <c r="BB8" s="21">
         <v>22163</v>
       </c>
-      <c r="BC8" s="22">
+      <c r="BC8" s="21">
         <v>9282</v>
       </c>
-      <c r="BD8" s="23">
+      <c r="BD8" s="22">
         <v>12881</v>
       </c>
-      <c r="BE8" s="22">
+      <c r="BE8" s="21">
         <v>28451</v>
       </c>
-      <c r="BF8" s="22">
+      <c r="BF8" s="21">
         <v>12734</v>
       </c>
-      <c r="BG8" s="23">
+      <c r="BG8" s="22">
         <v>15717</v>
       </c>
-      <c r="BH8" s="22">
+      <c r="BH8" s="21">
         <v>40751</v>
       </c>
-      <c r="BI8" s="22">
+      <c r="BI8" s="21">
         <v>17941</v>
       </c>
-      <c r="BJ8" s="23">
+      <c r="BJ8" s="22">
         <v>22810</v>
       </c>
     </row>
@@ -2167,375 +2148,375 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>150383</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>55878</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>94505</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>151267</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>57464</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>93803</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>150762</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>58499</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>92263</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>122058</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>57099</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="8">
         <v>64959</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <v>155812</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="7">
         <v>64924</v>
       </c>
-      <c r="P9" s="9">
+      <c r="P9" s="8">
         <v>90888</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="6">
         <v>175865</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9" s="7">
         <v>70478</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="8">
         <v>105387</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="6">
         <v>169031</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U9" s="7">
         <v>70178</v>
       </c>
-      <c r="V9" s="9">
+      <c r="V9" s="8">
         <v>98853</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="6">
         <v>186726</v>
       </c>
-      <c r="X9" s="8">
+      <c r="X9" s="7">
         <v>72157</v>
       </c>
-      <c r="Y9" s="9">
+      <c r="Y9" s="8">
         <v>114569</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="Z9" s="9">
         <v>208996</v>
       </c>
-      <c r="AA9" s="8">
+      <c r="AA9" s="7">
         <v>75243</v>
       </c>
-      <c r="AB9" s="9">
+      <c r="AB9" s="8">
         <v>133753</v>
       </c>
-      <c r="AC9" s="7">
+      <c r="AC9" s="6">
         <v>246851</v>
       </c>
-      <c r="AD9" s="8">
+      <c r="AD9" s="7">
         <v>71650</v>
       </c>
-      <c r="AE9" s="9">
+      <c r="AE9" s="8">
         <v>175201</v>
       </c>
-      <c r="AF9" s="16">
+      <c r="AF9" s="15">
         <v>465205</v>
       </c>
-      <c r="AG9" s="22">
+      <c r="AG9" s="21">
         <v>275560</v>
       </c>
-      <c r="AH9" s="22">
+      <c r="AH9" s="21">
         <v>129661</v>
       </c>
-      <c r="AI9" s="23">
+      <c r="AI9" s="22">
         <v>145899</v>
       </c>
-      <c r="AJ9" s="22">
+      <c r="AJ9" s="21">
         <v>287462</v>
       </c>
-      <c r="AK9" s="22">
+      <c r="AK9" s="21">
         <v>145539</v>
       </c>
-      <c r="AL9" s="23">
+      <c r="AL9" s="22">
         <v>141923</v>
       </c>
-      <c r="AM9" s="22">
+      <c r="AM9" s="21">
         <v>300496</v>
       </c>
-      <c r="AN9" s="22">
+      <c r="AN9" s="21">
         <v>151337</v>
       </c>
-      <c r="AO9" s="23">
+      <c r="AO9" s="22">
         <v>149159</v>
       </c>
-      <c r="AP9" s="22">
+      <c r="AP9" s="21">
         <v>306902</v>
       </c>
-      <c r="AQ9" s="22">
+      <c r="AQ9" s="21">
         <v>146170</v>
       </c>
-      <c r="AR9" s="23">
+      <c r="AR9" s="22">
         <v>160732</v>
       </c>
-      <c r="AS9" s="22">
+      <c r="AS9" s="21">
         <v>265086</v>
       </c>
-      <c r="AT9" s="22">
+      <c r="AT9" s="21">
         <v>123202</v>
       </c>
-      <c r="AU9" s="23">
+      <c r="AU9" s="22">
         <v>141884</v>
       </c>
-      <c r="AV9" s="22">
+      <c r="AV9" s="21">
         <v>233222</v>
       </c>
-      <c r="AW9" s="22">
+      <c r="AW9" s="21">
         <v>86771</v>
       </c>
-      <c r="AX9" s="23">
+      <c r="AX9" s="22">
         <v>146451</v>
       </c>
-      <c r="AY9" s="22">
+      <c r="AY9" s="21">
         <v>236205</v>
       </c>
-      <c r="AZ9" s="22">
+      <c r="AZ9" s="21">
         <v>81751</v>
       </c>
-      <c r="BA9" s="23">
+      <c r="BA9" s="22">
         <v>154454</v>
       </c>
-      <c r="BB9" s="22">
+      <c r="BB9" s="21">
         <v>184106</v>
       </c>
-      <c r="BC9" s="22">
+      <c r="BC9" s="21">
         <v>74202</v>
       </c>
-      <c r="BD9" s="23">
+      <c r="BD9" s="22">
         <v>109904</v>
       </c>
-      <c r="BE9" s="22">
+      <c r="BE9" s="21">
         <v>209334</v>
       </c>
-      <c r="BF9" s="22">
+      <c r="BF9" s="21">
         <v>90403</v>
       </c>
-      <c r="BG9" s="23">
+      <c r="BG9" s="22">
         <v>118931</v>
       </c>
-      <c r="BH9" s="22">
+      <c r="BH9" s="21">
         <v>215205</v>
       </c>
-      <c r="BI9" s="22">
+      <c r="BI9" s="21">
         <v>84350</v>
       </c>
-      <c r="BJ9" s="23">
+      <c r="BJ9" s="22">
         <v>130855</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="30">
+      <c r="A10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="28">
         <v>444</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <v>259</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="30">
         <v>185</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="28">
         <v>513</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="29">
         <v>263</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="30">
         <v>250</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="28">
         <v>526</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="29">
         <v>256</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="30">
         <v>270</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="28">
         <v>468</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="29">
         <v>250</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="30">
         <v>218</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="28">
         <v>820</v>
       </c>
-      <c r="O10" s="31">
+      <c r="O10" s="29">
         <v>324</v>
       </c>
-      <c r="P10" s="32">
+      <c r="P10" s="30">
         <v>496</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="Q10" s="28">
         <v>947</v>
       </c>
-      <c r="R10" s="31">
+      <c r="R10" s="29">
         <v>410</v>
       </c>
-      <c r="S10" s="32">
+      <c r="S10" s="30">
         <v>537</v>
       </c>
-      <c r="T10" s="30">
+      <c r="T10" s="28">
         <v>1292</v>
       </c>
-      <c r="U10" s="31">
+      <c r="U10" s="29">
         <v>357</v>
       </c>
-      <c r="V10" s="32">
+      <c r="V10" s="30">
         <v>935</v>
       </c>
-      <c r="W10" s="30">
+      <c r="W10" s="28">
         <v>2446</v>
       </c>
-      <c r="X10" s="31">
+      <c r="X10" s="29">
         <v>593</v>
       </c>
-      <c r="Y10" s="32">
+      <c r="Y10" s="30">
         <v>1853</v>
       </c>
-      <c r="Z10" s="30">
+      <c r="Z10" s="28">
         <v>2307</v>
       </c>
-      <c r="AA10" s="31">
+      <c r="AA10" s="29">
         <v>498</v>
       </c>
-      <c r="AB10" s="32">
+      <c r="AB10" s="30">
         <v>1809</v>
       </c>
-      <c r="AC10" s="30">
+      <c r="AC10" s="28">
         <v>2250</v>
       </c>
-      <c r="AD10" s="31">
+      <c r="AD10" s="29">
         <v>495</v>
       </c>
-      <c r="AE10" s="32">
+      <c r="AE10" s="30">
         <v>1755</v>
       </c>
-      <c r="AF10" s="28">
+      <c r="AF10" s="26">
         <v>167</v>
       </c>
-      <c r="AG10" s="26">
+      <c r="AG10" s="24">
         <v>1868</v>
       </c>
-      <c r="AH10" s="26">
+      <c r="AH10" s="24">
         <v>805</v>
       </c>
-      <c r="AI10" s="27">
+      <c r="AI10" s="25">
         <v>1063</v>
       </c>
-      <c r="AJ10" s="26">
+      <c r="AJ10" s="24">
         <v>1571</v>
       </c>
-      <c r="AK10" s="26">
+      <c r="AK10" s="24">
         <v>712</v>
       </c>
-      <c r="AL10" s="27">
+      <c r="AL10" s="25">
         <v>859</v>
       </c>
-      <c r="AM10" s="26">
+      <c r="AM10" s="24">
         <v>1426</v>
       </c>
-      <c r="AN10" s="26">
+      <c r="AN10" s="24">
         <v>729</v>
       </c>
-      <c r="AO10" s="27">
+      <c r="AO10" s="25">
         <v>697</v>
       </c>
-      <c r="AP10" s="26">
+      <c r="AP10" s="24">
         <v>1339</v>
       </c>
-      <c r="AQ10" s="26">
+      <c r="AQ10" s="24">
         <v>692</v>
       </c>
-      <c r="AR10" s="27">
+      <c r="AR10" s="25">
         <v>647</v>
       </c>
-      <c r="AS10" s="26">
+      <c r="AS10" s="24">
         <v>1318</v>
       </c>
-      <c r="AT10" s="26">
+      <c r="AT10" s="24">
         <v>643</v>
       </c>
-      <c r="AU10" s="27">
+      <c r="AU10" s="25">
         <v>675</v>
       </c>
-      <c r="AV10" s="26">
+      <c r="AV10" s="24">
         <v>930</v>
       </c>
-      <c r="AW10" s="26">
+      <c r="AW10" s="24">
         <v>440</v>
       </c>
-      <c r="AX10" s="27">
+      <c r="AX10" s="25">
         <v>490</v>
       </c>
-      <c r="AY10" s="26">
+      <c r="AY10" s="24">
         <v>882</v>
       </c>
-      <c r="AZ10" s="26">
+      <c r="AZ10" s="24">
         <v>392</v>
       </c>
-      <c r="BA10" s="27">
+      <c r="BA10" s="25">
         <v>490</v>
       </c>
-      <c r="BB10" s="26">
+      <c r="BB10" s="24">
         <v>906</v>
       </c>
-      <c r="BC10" s="26">
+      <c r="BC10" s="24">
         <v>379</v>
       </c>
-      <c r="BD10" s="27">
+      <c r="BD10" s="25">
         <v>527</v>
       </c>
-      <c r="BE10" s="26">
+      <c r="BE10" s="24">
         <v>964</v>
       </c>
-      <c r="BF10" s="26">
+      <c r="BF10" s="24">
         <v>568</v>
       </c>
-      <c r="BG10" s="27">
+      <c r="BG10" s="25">
         <v>396</v>
       </c>
-      <c r="BH10" s="26">
+      <c r="BH10" s="24">
         <v>2268</v>
       </c>
-      <c r="BI10" s="26">
+      <c r="BI10" s="24">
         <v>1058</v>
       </c>
-      <c r="BJ10" s="27">
+      <c r="BJ10" s="25">
         <v>1210</v>
       </c>
     </row>
@@ -2543,187 +2524,187 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>169</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>130</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>39</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>154</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>110</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>44</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>157</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>109</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>48</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>163</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="7">
         <v>109</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="8">
         <v>54</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="6">
         <v>162</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="7">
         <v>102</v>
       </c>
-      <c r="P11" s="9">
+      <c r="P11" s="8">
         <v>60</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="6">
         <v>188</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11" s="7">
         <v>128</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11" s="8">
         <v>60</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="6">
         <v>187</v>
       </c>
-      <c r="U11" s="8">
+      <c r="U11" s="7">
         <v>124</v>
       </c>
-      <c r="V11" s="9">
+      <c r="V11" s="8">
         <v>63</v>
       </c>
-      <c r="W11" s="7">
+      <c r="W11" s="6">
         <v>209</v>
       </c>
-      <c r="X11" s="8">
+      <c r="X11" s="7">
         <v>117</v>
       </c>
-      <c r="Y11" s="9">
+      <c r="Y11" s="8">
         <v>92</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="Z11" s="6">
         <v>185</v>
       </c>
-      <c r="AA11" s="8">
+      <c r="AA11" s="7">
         <v>102</v>
       </c>
-      <c r="AB11" s="9">
+      <c r="AB11" s="8">
         <v>83</v>
       </c>
-      <c r="AC11" s="7">
+      <c r="AC11" s="6">
         <v>192</v>
       </c>
-      <c r="AD11" s="8">
+      <c r="AD11" s="7">
         <v>100</v>
       </c>
-      <c r="AE11" s="9">
+      <c r="AE11" s="8">
         <v>92</v>
       </c>
-      <c r="AF11" s="16">
+      <c r="AF11" s="15">
         <v>116</v>
       </c>
-      <c r="AG11" s="22">
+      <c r="AG11" s="21">
         <v>190</v>
       </c>
-      <c r="AH11" s="22">
+      <c r="AH11" s="21">
         <v>124</v>
       </c>
-      <c r="AI11" s="23">
+      <c r="AI11" s="22">
         <v>66</v>
       </c>
-      <c r="AJ11" s="22">
+      <c r="AJ11" s="21">
         <v>148</v>
       </c>
-      <c r="AK11" s="22">
+      <c r="AK11" s="21">
         <v>96</v>
       </c>
-      <c r="AL11" s="23">
+      <c r="AL11" s="22">
         <v>52</v>
       </c>
-      <c r="AM11" s="22">
+      <c r="AM11" s="21">
         <v>129</v>
       </c>
-      <c r="AN11" s="22">
+      <c r="AN11" s="21">
         <v>94</v>
       </c>
-      <c r="AO11" s="23">
+      <c r="AO11" s="22">
         <v>35</v>
       </c>
-      <c r="AP11" s="22">
+      <c r="AP11" s="21">
         <v>122</v>
       </c>
-      <c r="AQ11" s="22">
+      <c r="AQ11" s="21">
         <v>82</v>
       </c>
-      <c r="AR11" s="23">
+      <c r="AR11" s="22">
         <v>40</v>
       </c>
-      <c r="AS11" s="22">
+      <c r="AS11" s="21">
         <v>91</v>
       </c>
-      <c r="AT11" s="22">
+      <c r="AT11" s="21">
         <v>56</v>
       </c>
-      <c r="AU11" s="23">
+      <c r="AU11" s="22">
         <v>35</v>
       </c>
-      <c r="AV11" s="22">
+      <c r="AV11" s="21">
         <v>102</v>
       </c>
-      <c r="AW11" s="22">
+      <c r="AW11" s="21">
         <v>57</v>
       </c>
-      <c r="AX11" s="23">
+      <c r="AX11" s="22">
         <v>45</v>
       </c>
-      <c r="AY11" s="22">
+      <c r="AY11" s="21">
         <v>83</v>
       </c>
-      <c r="AZ11" s="22">
+      <c r="AZ11" s="21">
         <v>54</v>
       </c>
-      <c r="BA11" s="23">
+      <c r="BA11" s="22">
         <v>29</v>
       </c>
-      <c r="BB11" s="22">
+      <c r="BB11" s="21">
         <v>94</v>
       </c>
-      <c r="BC11" s="22">
+      <c r="BC11" s="21">
         <v>52</v>
       </c>
-      <c r="BD11" s="23">
+      <c r="BD11" s="22">
         <v>42</v>
       </c>
-      <c r="BE11" s="22">
+      <c r="BE11" s="21">
         <v>91</v>
       </c>
-      <c r="BF11" s="22">
+      <c r="BF11" s="21">
         <v>86</v>
       </c>
-      <c r="BG11" s="23">
+      <c r="BG11" s="22">
         <v>5</v>
       </c>
-      <c r="BH11" s="22">
+      <c r="BH11" s="21">
         <v>102</v>
       </c>
-      <c r="BI11" s="22">
+      <c r="BI11" s="21">
         <v>95</v>
       </c>
-      <c r="BJ11" s="23">
+      <c r="BJ11" s="22">
         <v>7</v>
       </c>
     </row>
@@ -2752,166 +2733,38 @@
       <c r="AD16"/>
       <c r="AE16"/>
     </row>
-    <row r="17" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC17"/>
-      <c r="AD17"/>
-      <c r="AE17"/>
-    </row>
-    <row r="18" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC18"/>
-      <c r="AD18"/>
-      <c r="AE18"/>
-    </row>
-    <row r="19" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC19"/>
-      <c r="AD19"/>
-      <c r="AE19"/>
-    </row>
-    <row r="20" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC20"/>
-      <c r="AD20"/>
-      <c r="AE20"/>
-    </row>
-    <row r="21" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC21"/>
-      <c r="AD21"/>
-      <c r="AE21"/>
-    </row>
-    <row r="22" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC22"/>
-      <c r="AD22"/>
-      <c r="AE22"/>
-    </row>
-    <row r="23" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC23"/>
-      <c r="AD23"/>
-      <c r="AE23"/>
-    </row>
-    <row r="24" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC24"/>
-      <c r="AD24"/>
-      <c r="AE24"/>
-    </row>
-    <row r="25" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC25"/>
-      <c r="AD25"/>
-      <c r="AE25"/>
-    </row>
-    <row r="26" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC26"/>
-      <c r="AD26"/>
-      <c r="AE26"/>
-    </row>
-    <row r="27" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC27"/>
-      <c r="AD27"/>
-      <c r="AE27"/>
-    </row>
-    <row r="28" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC28"/>
-      <c r="AD28"/>
-      <c r="AE28"/>
-    </row>
-    <row r="29" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC29"/>
-      <c r="AD29"/>
-      <c r="AE29"/>
-    </row>
-    <row r="30" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC30"/>
-      <c r="AD30"/>
-      <c r="AE30"/>
-    </row>
-    <row r="31" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC31"/>
-      <c r="AD31"/>
-      <c r="AE31"/>
-    </row>
-    <row r="32" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32"/>
-    </row>
-    <row r="33" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-    </row>
-    <row r="34" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-    </row>
-    <row r="35" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-    </row>
-    <row r="36" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-    </row>
-    <row r="37" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-    </row>
-    <row r="38" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC38"/>
-      <c r="AD38"/>
-      <c r="AE38"/>
-    </row>
-    <row r="39" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC39"/>
-      <c r="AD39"/>
-      <c r="AE39"/>
-    </row>
-    <row r="40" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC40"/>
-      <c r="AD40"/>
-      <c r="AE40"/>
-    </row>
-    <row r="41" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC41"/>
-      <c r="AD41"/>
-      <c r="AE41"/>
-    </row>
-    <row r="42" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC42"/>
-      <c r="AD42"/>
-      <c r="AE42"/>
-    </row>
-    <row r="43" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC43"/>
-      <c r="AD43"/>
-      <c r="AE43"/>
-    </row>
-    <row r="44" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC44"/>
-      <c r="AD44"/>
-      <c r="AE44"/>
-    </row>
-    <row r="45" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC45"/>
-      <c r="AD45"/>
-      <c r="AE45"/>
-    </row>
-    <row r="46" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC46"/>
-      <c r="AD46"/>
-      <c r="AE46"/>
-    </row>
-    <row r="47" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC47"/>
-      <c r="AD47"/>
-      <c r="AE47"/>
-    </row>
-    <row r="48" spans="29:31" x14ac:dyDescent="0.25">
-      <c r="AC48"/>
-      <c r="AD48"/>
-      <c r="AE48"/>
-    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="8:31" x14ac:dyDescent="0.25">
       <c r="AC49"/>
       <c r="AD49"/>
@@ -3013,26 +2866,26 @@
     <row r="71" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="AV1:AX1"/>
+    <mergeCell ref="AY1:BA1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="BE1:BG1"/>
+    <mergeCell ref="BH1:BJ1"/>
     <mergeCell ref="AG1:AI1"/>
     <mergeCell ref="AJ1:AL1"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="AP1:AR1"/>
     <mergeCell ref="AS1:AU1"/>
-    <mergeCell ref="AV1:AX1"/>
-    <mergeCell ref="AY1:BA1"/>
-    <mergeCell ref="BB1:BD1"/>
-    <mergeCell ref="BE1:BG1"/>
-    <mergeCell ref="BH1:BJ1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>